<commit_message>
Successfully functional!!!! Version 1.0!
</commit_message>
<xml_diff>
--- a/Pokemon.xlsx
+++ b/Pokemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijan Badhya\Documents\Pokemon_elite_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE84779A-FEB1-477D-8C19-8FD13E5B221A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9224F31-BB7C-468E-A7FE-2B510CBD5C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2718,8 +2718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CD488"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H66" workbookViewId="0">
-      <selection activeCell="P74" sqref="P74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
End of the List
</commit_message>
<xml_diff>
--- a/Pokemon.xlsx
+++ b/Pokemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijan Badhya\Documents\Pokemon_elite_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708A28B6-394D-4B92-9676-75E3331E7675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC802FC5-90E4-4683-AD02-12482EE84182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$Q$1:$Q$490</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$Q$1:$Q$489</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15154" uniqueCount="812">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15353" uniqueCount="812">
   <si>
     <t>Name</t>
   </si>
@@ -2224,9 +2224,6 @@
     <t>Zebstrika</t>
   </si>
   <si>
-    <t>Zeraora</t>
-  </si>
-  <si>
     <t>Zoroark</t>
   </si>
   <si>
@@ -2459,6 +2456,9 @@
   </si>
   <si>
     <t>Skeledirge</t>
+  </si>
+  <si>
+    <t>Bite</t>
   </si>
 </sst>
 </file>
@@ -2844,10 +2844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CN490"/>
+  <dimension ref="A1:CN489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM278" zoomScale="99" workbookViewId="0">
-      <selection activeCell="AR290" sqref="AR290"/>
+    <sheetView tabSelected="1" topLeftCell="R375" zoomScale="99" workbookViewId="0">
+      <selection activeCell="AI392" sqref="AI392"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3100,34 +3100,34 @@
         <v>81</v>
       </c>
       <c r="CE1" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="CF1" s="2" t="s">
         <v>791</v>
       </c>
-      <c r="CF1" s="2" t="s">
+      <c r="CG1" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="CH1" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="CI1" s="2" t="s">
+        <v>793</v>
+      </c>
+      <c r="CJ1" s="2" t="s">
         <v>792</v>
       </c>
-      <c r="CG1" s="2" t="s">
-        <v>791</v>
-      </c>
-      <c r="CH1" s="2" t="s">
-        <v>790</v>
-      </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CK1" s="2" t="s">
         <v>794</v>
       </c>
-      <c r="CJ1" s="2" t="s">
-        <v>793</v>
-      </c>
-      <c r="CK1" s="2" t="s">
+      <c r="CL1" s="2" t="s">
         <v>795</v>
       </c>
-      <c r="CL1" s="2" t="s">
+      <c r="CM1" s="2" t="s">
         <v>796</v>
       </c>
-      <c r="CM1" s="2" t="s">
+      <c r="CN1" s="2" t="s">
         <v>797</v>
-      </c>
-      <c r="CN1" s="2" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="2" spans="1:92" x14ac:dyDescent="0.35">
@@ -4054,7 +4054,7 @@
     </row>
     <row r="10" spans="1:92" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B10" t="s">
         <v>83</v>
@@ -4512,7 +4512,7 @@
         <v>102</v>
       </c>
       <c r="BI14" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="BJ14" t="s">
         <v>89</v>
@@ -6728,7 +6728,7 @@
         <v>89</v>
       </c>
       <c r="AK39" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="AL39" t="s">
         <v>122</v>
@@ -7594,7 +7594,7 @@
         <v>83</v>
       </c>
       <c r="AE49" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="AF49" t="s">
         <v>89</v>
@@ -10111,7 +10111,7 @@
         <v>95</v>
       </c>
       <c r="Y82" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="Z82" t="s">
         <v>122</v>
@@ -10464,7 +10464,7 @@
         <v>122</v>
       </c>
       <c r="AC86" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="AD86" t="s">
         <v>84</v>
@@ -10472,7 +10472,7 @@
     </row>
     <row r="87" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B87" t="s">
         <v>97</v>
@@ -10583,7 +10583,7 @@
         <v>129</v>
       </c>
       <c r="AQ87" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="AR87" t="s">
         <v>84</v>
@@ -11158,7 +11158,7 @@
         <v>83</v>
       </c>
       <c r="AC94" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="AD94" t="s">
         <v>83</v>
@@ -11366,7 +11366,7 @@
         <v>95</v>
       </c>
       <c r="BE96" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="BF96" t="s">
         <v>84</v>
@@ -11597,7 +11597,7 @@
         <v>89</v>
       </c>
       <c r="S99" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="T99" t="s">
         <v>87</v>
@@ -11683,13 +11683,13 @@
         <v>85</v>
       </c>
       <c r="I100" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="J100" t="s">
         <v>116</v>
       </c>
       <c r="K100" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="L100" t="s">
         <v>116</v>
@@ -11784,13 +11784,13 @@
         <v>148</v>
       </c>
       <c r="I101" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="J101" t="s">
         <v>116</v>
       </c>
       <c r="K101" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="L101" t="s">
         <v>116</v>
@@ -12001,7 +12001,7 @@
         <v>102</v>
       </c>
       <c r="AK103" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="AL103" t="s">
         <v>89</v>
@@ -12178,7 +12178,7 @@
     </row>
     <row r="106" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B106" t="s">
         <v>110</v>
@@ -12265,7 +12265,7 @@
         <v>84</v>
       </c>
       <c r="AI106" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="AJ106" t="s">
         <v>92</v>
@@ -12654,7 +12654,7 @@
         <v>87</v>
       </c>
       <c r="S110" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="T110" t="s">
         <v>87</v>
@@ -12814,7 +12814,7 @@
         <v>87</v>
       </c>
       <c r="K112" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="L112" t="s">
         <v>87</v>
@@ -13014,7 +13014,7 @@
         <v>119</v>
       </c>
       <c r="BA113" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="BB113" t="s">
         <v>102</v>
@@ -13026,7 +13026,7 @@
         <v>95</v>
       </c>
       <c r="BE113" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="BF113" t="s">
         <v>84</v>
@@ -13204,7 +13204,7 @@
         <v>129</v>
       </c>
       <c r="AG115" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="AH115" t="s">
         <v>129</v>
@@ -13216,7 +13216,7 @@
         <v>129</v>
       </c>
       <c r="AK115" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="AL115" t="s">
         <v>129</v>
@@ -13320,7 +13320,7 @@
         <v>119</v>
       </c>
       <c r="AK116" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AL116" t="s">
         <v>116</v>
@@ -13400,7 +13400,7 @@
         <v>129</v>
       </c>
       <c r="O117" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="P117" t="s">
         <v>106</v>
@@ -13558,7 +13558,7 @@
         <v>89</v>
       </c>
       <c r="AG118" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="AH118" t="s">
         <v>102</v>
@@ -14400,7 +14400,7 @@
         <v>95</v>
       </c>
       <c r="AG125" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="AH125" t="s">
         <v>122</v>
@@ -14420,7 +14420,7 @@
         <v>85</v>
       </c>
       <c r="I126" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="J126" t="s">
         <v>122</v>
@@ -14941,7 +14941,7 @@
         <v>92</v>
       </c>
       <c r="W130" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="X130" t="s">
         <v>129</v>
@@ -14965,7 +14965,7 @@
         <v>129</v>
       </c>
       <c r="AE130" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="AF130" t="s">
         <v>129</v>
@@ -15035,7 +15035,7 @@
         <v>89</v>
       </c>
       <c r="U132" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="V132" t="s">
         <v>87</v>
@@ -15447,7 +15447,7 @@
         <v>84</v>
       </c>
       <c r="Q137" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="R137" t="s">
         <v>116</v>
@@ -15543,7 +15543,7 @@
         <v>84</v>
       </c>
       <c r="AW137" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="AX137" t="s">
         <v>102</v>
@@ -15774,7 +15774,7 @@
         <v>83</v>
       </c>
       <c r="Y140" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="Z140" t="s">
         <v>129</v>
@@ -15981,7 +15981,7 @@
         <v>87</v>
       </c>
       <c r="AE143" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="AF143" t="s">
         <v>110</v>
@@ -16082,7 +16082,7 @@
         <v>89</v>
       </c>
       <c r="AC144" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="AD144" t="s">
         <v>87</v>
@@ -16219,13 +16219,13 @@
         <v>106</v>
       </c>
       <c r="M145" t="s">
+        <v>755</v>
+      </c>
+      <c r="N145" t="s">
+        <v>89</v>
+      </c>
+      <c r="O145" t="s">
         <v>756</v>
-      </c>
-      <c r="N145" t="s">
-        <v>89</v>
-      </c>
-      <c r="O145" t="s">
-        <v>757</v>
       </c>
       <c r="P145" t="s">
         <v>106</v>
@@ -16311,13 +16311,13 @@
         <v>85</v>
       </c>
       <c r="I146" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="J146" t="s">
         <v>116</v>
       </c>
       <c r="K146" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="L146" t="s">
         <v>83</v>
@@ -16341,13 +16341,13 @@
         <v>117</v>
       </c>
       <c r="S146" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="T146" t="s">
         <v>106</v>
       </c>
       <c r="U146" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="V146" t="s">
         <v>83</v>
@@ -16742,7 +16742,7 @@
         <v>85</v>
       </c>
       <c r="I150" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="J150" t="s">
         <v>116</v>
@@ -16760,7 +16760,7 @@
         <v>117</v>
       </c>
       <c r="O150" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="P150" t="s">
         <v>116</v>
@@ -16896,7 +16896,7 @@
         <v>92</v>
       </c>
       <c r="K152" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="L152" t="s">
         <v>116</v>
@@ -16934,7 +16934,7 @@
     </row>
     <row r="153" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B153" t="s">
         <v>117</v>
@@ -17115,7 +17115,7 @@
         <v>83</v>
       </c>
       <c r="K155" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="L155" t="s">
         <v>83</v>
@@ -17133,7 +17133,7 @@
         <v>83</v>
       </c>
       <c r="Q155" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="R155" t="s">
         <v>83</v>
@@ -17163,7 +17163,7 @@
         <v>83</v>
       </c>
       <c r="AA155" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="AB155" t="s">
         <v>110</v>
@@ -17204,7 +17204,7 @@
         <v>83</v>
       </c>
       <c r="M156" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="N156" t="s">
         <v>117</v>
@@ -17234,13 +17234,13 @@
         <v>117</v>
       </c>
       <c r="W156" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="X156" t="s">
         <v>106</v>
       </c>
       <c r="Y156" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="Z156" t="s">
         <v>106</v>
@@ -17252,7 +17252,7 @@
         <v>117</v>
       </c>
       <c r="AC156" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AD156" t="s">
         <v>116</v>
@@ -17294,7 +17294,7 @@
         <v>83</v>
       </c>
       <c r="AQ156" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="AR156" t="s">
         <v>110</v>
@@ -17864,7 +17864,7 @@
         <v>102</v>
       </c>
       <c r="K162" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="L162" t="s">
         <v>83</v>
@@ -17900,7 +17900,7 @@
         <v>119</v>
       </c>
       <c r="W162" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="X162" t="s">
         <v>83</v>
@@ -17984,7 +17984,7 @@
         <v>106</v>
       </c>
       <c r="AY162" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="AZ162" t="s">
         <v>129</v>
@@ -18382,7 +18382,7 @@
         <v>106</v>
       </c>
       <c r="AA166" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="AB166" t="s">
         <v>127</v>
@@ -18544,7 +18544,7 @@
     </row>
     <row r="169" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B169" t="s">
         <v>84</v>
@@ -18934,7 +18934,7 @@
         <v>84</v>
       </c>
       <c r="AU172" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="AV172" t="s">
         <v>110</v>
@@ -18964,7 +18964,7 @@
         <v>87</v>
       </c>
       <c r="BE172" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="BF172" t="s">
         <v>89</v>
@@ -19044,7 +19044,7 @@
         <v>117</v>
       </c>
       <c r="Y173" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="Z173" t="s">
         <v>87</v>
@@ -19098,7 +19098,7 @@
         <v>102</v>
       </c>
       <c r="AQ173" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="AR173" t="s">
         <v>106</v>
@@ -19202,7 +19202,7 @@
         <v>117</v>
       </c>
       <c r="AK174" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="AL174" t="s">
         <v>106</v>
@@ -19428,7 +19428,7 @@
         <v>83</v>
       </c>
       <c r="AE176" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="AF176" t="s">
         <v>87</v>
@@ -19464,7 +19464,7 @@
         <v>119</v>
       </c>
       <c r="AQ176" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AR176" t="s">
         <v>116</v>
@@ -20276,7 +20276,7 @@
         <v>129</v>
       </c>
       <c r="Q183" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="R183" t="s">
         <v>129</v>
@@ -20324,7 +20324,7 @@
         <v>129</v>
       </c>
       <c r="AG183" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="AH183" t="s">
         <v>129</v>
@@ -20505,7 +20505,7 @@
         <v>87</v>
       </c>
       <c r="Q185" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="R185" t="s">
         <v>87</v>
@@ -20985,7 +20985,7 @@
         <v>127</v>
       </c>
       <c r="S188" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="T188" t="s">
         <v>87</v>
@@ -21069,7 +21069,7 @@
         <v>97</v>
       </c>
       <c r="AU188" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="AV188" t="s">
         <v>106</v>
@@ -21104,7 +21104,7 @@
         <v>102</v>
       </c>
       <c r="K189" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="L189" t="s">
         <v>89</v>
@@ -21224,7 +21224,7 @@
         <v>102</v>
       </c>
       <c r="AY189" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="AZ189" t="s">
         <v>92</v>
@@ -21688,7 +21688,7 @@
         <v>95</v>
       </c>
       <c r="AG193" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="AH193" t="s">
         <v>92</v>
@@ -21735,7 +21735,7 @@
         <v>95</v>
       </c>
       <c r="O194" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="P194" t="s">
         <v>117</v>
@@ -21795,7 +21795,7 @@
         <v>95</v>
       </c>
       <c r="AI194" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="AJ194" t="s">
         <v>92</v>
@@ -21884,7 +21884,7 @@
         <v>116</v>
       </c>
       <c r="AC195" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="AD195" t="s">
         <v>102</v>
@@ -21902,7 +21902,7 @@
         <v>102</v>
       </c>
       <c r="AI195" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="AJ195" t="s">
         <v>92</v>
@@ -21934,7 +21934,7 @@
         <v>85</v>
       </c>
       <c r="I196" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="J196" t="s">
         <v>122</v>
@@ -21964,7 +21964,7 @@
         <v>97</v>
       </c>
       <c r="S196" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="T196" t="s">
         <v>110</v>
@@ -22142,7 +22142,7 @@
         <v>122</v>
       </c>
       <c r="K198" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="L198" t="s">
         <v>122</v>
@@ -23015,7 +23015,7 @@
         <v>116</v>
       </c>
       <c r="AE207" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="AF207" t="s">
         <v>84</v>
@@ -23027,7 +23027,7 @@
         <v>87</v>
       </c>
       <c r="AI207" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="AJ207" t="s">
         <v>84</v>
@@ -23071,7 +23071,7 @@
         <v>100</v>
       </c>
       <c r="O208" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="P208" t="s">
         <v>117</v>
@@ -23706,7 +23706,7 @@
         <v>89</v>
       </c>
       <c r="AA215" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="AB215" t="s">
         <v>87</v>
@@ -24125,13 +24125,13 @@
         <v>87</v>
       </c>
       <c r="M219" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="N219" t="s">
         <v>87</v>
       </c>
       <c r="O219" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="P219" t="s">
         <v>89</v>
@@ -24223,7 +24223,7 @@
         <v>129</v>
       </c>
       <c r="O220" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="P220" t="s">
         <v>89</v>
@@ -24297,7 +24297,7 @@
     </row>
     <row r="221" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B221" t="s">
         <v>106</v>
@@ -24534,7 +24534,7 @@
         <v>87</v>
       </c>
       <c r="S224" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="T224" t="s">
         <v>83</v>
@@ -25013,7 +25013,7 @@
         <v>92</v>
       </c>
       <c r="AO228" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="AP228" t="s">
         <v>110</v>
@@ -25087,7 +25087,7 @@
         <v>119</v>
       </c>
       <c r="W229" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="X229" t="s">
         <v>116</v>
@@ -25117,7 +25117,7 @@
         <v>97</v>
       </c>
       <c r="AG229" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="AH229" t="s">
         <v>129</v>
@@ -25390,7 +25390,7 @@
         <v>110</v>
       </c>
       <c r="AI232" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="AJ232" t="s">
         <v>87</v>
@@ -25410,7 +25410,7 @@
         <v>121</v>
       </c>
       <c r="J233" t="s">
-        <v>87</v>
+        <v>122</v>
       </c>
       <c r="K233" t="s">
         <v>199</v>
@@ -25461,7 +25461,7 @@
         <v>89</v>
       </c>
       <c r="AA233" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="AB233" t="s">
         <v>87</v>
@@ -25841,7 +25841,7 @@
         <v>87</v>
       </c>
       <c r="M237" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="N237" t="s">
         <v>87</v>
@@ -25897,7 +25897,7 @@
         <v>87</v>
       </c>
       <c r="M238" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="N238" t="s">
         <v>87</v>
@@ -25945,7 +25945,7 @@
         <v>92</v>
       </c>
       <c r="AC238" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="AD238" t="s">
         <v>87</v>
@@ -25975,7 +25975,7 @@
         <v>116</v>
       </c>
       <c r="AM238" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="AN238" t="s">
         <v>87</v>
@@ -26091,7 +26091,7 @@
         <v>110</v>
       </c>
       <c r="Q239" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="R239" t="s">
         <v>117</v>
@@ -26175,7 +26175,7 @@
         <v>102</v>
       </c>
       <c r="AS239" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="AT239" t="s">
         <v>89</v>
@@ -27071,7 +27071,7 @@
         <v>85</v>
       </c>
       <c r="I249" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="J249" t="s">
         <v>122</v>
@@ -27160,7 +27160,7 @@
         <v>92</v>
       </c>
       <c r="O250" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="P250" t="s">
         <v>117</v>
@@ -27262,7 +27262,7 @@
         <v>102</v>
       </c>
       <c r="AW250" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="AX250" t="s">
         <v>92</v>
@@ -27476,7 +27476,7 @@
         <v>95</v>
       </c>
       <c r="BA252" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="BB252" t="s">
         <v>87</v>
@@ -27606,7 +27606,7 @@
         <v>95</v>
       </c>
       <c r="S254" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="T254" t="s">
         <v>89</v>
@@ -27659,7 +27659,7 @@
         <v>106</v>
       </c>
       <c r="U255" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="V255" t="s">
         <v>117</v>
@@ -28099,7 +28099,7 @@
         <v>102</v>
       </c>
       <c r="BC259" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="BD259" t="s">
         <v>89</v>
@@ -28117,13 +28117,13 @@
         <v>95</v>
       </c>
       <c r="BI259" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="BJ259" t="s">
         <v>89</v>
       </c>
       <c r="BK259" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="BL259" t="s">
         <v>89</v>
@@ -28197,7 +28197,7 @@
         <v>97</v>
       </c>
       <c r="AA260" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="AB260" t="s">
         <v>129</v>
@@ -28321,7 +28321,7 @@
         <v>122</v>
       </c>
       <c r="K262" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="L262" t="s">
         <v>122</v>
@@ -28903,7 +28903,7 @@
     </row>
     <row r="268" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B268" t="s">
         <v>110</v>
@@ -29126,7 +29126,7 @@
         <v>89</v>
       </c>
       <c r="O270" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="P270" t="s">
         <v>87</v>
@@ -29429,7 +29429,7 @@
         <v>89</v>
       </c>
       <c r="AA273" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="AB273" t="s">
         <v>87</v>
@@ -29563,7 +29563,7 @@
         <v>102</v>
       </c>
       <c r="K274" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="L274" t="s">
         <v>83</v>
@@ -29788,7 +29788,7 @@
         <v>119</v>
       </c>
       <c r="O277" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="P277" t="s">
         <v>117</v>
@@ -29854,7 +29854,7 @@
         <v>117</v>
       </c>
       <c r="AK277" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="AL277" t="s">
         <v>110</v>
@@ -30406,7 +30406,7 @@
         <v>119</v>
       </c>
       <c r="O283" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="P283" t="s">
         <v>117</v>
@@ -30520,7 +30520,7 @@
         <v>102</v>
       </c>
       <c r="BA283" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="BB283" t="s">
         <v>89</v>
@@ -30701,7 +30701,7 @@
         <v>83</v>
       </c>
       <c r="O285" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="P285" t="s">
         <v>97</v>
@@ -30754,7 +30754,7 @@
         <v>92</v>
       </c>
       <c r="K286" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="L286" t="s">
         <v>108</v>
@@ -31685,7 +31685,7 @@
         <v>110</v>
       </c>
       <c r="W294" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="X294" t="s">
         <v>110</v>
@@ -31789,7 +31789,7 @@
         <v>87</v>
       </c>
       <c r="AG295" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="AH295" t="s">
         <v>110</v>
@@ -32208,7 +32208,7 @@
         <v>127</v>
       </c>
       <c r="K299" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="L299" t="s">
         <v>89</v>
@@ -32303,7 +32303,7 @@
         <v>127</v>
       </c>
       <c r="K300" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="L300" t="s">
         <v>89</v>
@@ -32419,7 +32419,7 @@
         <v>100</v>
       </c>
       <c r="Q301" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="R301" t="s">
         <v>89</v>
@@ -32882,7 +32882,7 @@
         <v>85</v>
       </c>
       <c r="I309" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="J309" t="s">
         <v>122</v>
@@ -32992,7 +32992,7 @@
         <v>97</v>
       </c>
       <c r="W310" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="X310" t="s">
         <v>129</v>
@@ -33606,7 +33606,7 @@
     </row>
     <row r="317" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B317" t="s">
         <v>129</v>
@@ -33683,7 +33683,7 @@
         <v>85</v>
       </c>
       <c r="I318" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="J318" t="s">
         <v>122</v>
@@ -33826,7 +33826,7 @@
         <v>127</v>
       </c>
       <c r="K319" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="L319" t="s">
         <v>83</v>
@@ -34197,7 +34197,7 @@
         <v>129</v>
       </c>
       <c r="Y323" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="Z323" t="s">
         <v>116</v>
@@ -34432,13 +34432,13 @@
         <v>102</v>
       </c>
       <c r="AI325" t="s">
+        <v>787</v>
+      </c>
+      <c r="AJ325" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK325" t="s">
         <v>788</v>
-      </c>
-      <c r="AJ325" t="s">
-        <v>87</v>
-      </c>
-      <c r="AK325" t="s">
-        <v>789</v>
       </c>
       <c r="AL325" t="s">
         <v>87</v>
@@ -34732,7 +34732,7 @@
         <v>102</v>
       </c>
       <c r="AI328" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="AJ328" t="s">
         <v>89</v>
@@ -34877,7 +34877,7 @@
         <v>97</v>
       </c>
       <c r="U330" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="V330" t="s">
         <v>110</v>
@@ -35434,7 +35434,7 @@
         <v>127</v>
       </c>
       <c r="M337" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="N337" t="s">
         <v>97</v>
@@ -35553,7 +35553,7 @@
         <v>129</v>
       </c>
       <c r="AA338" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AB338" t="s">
         <v>116</v>
@@ -35657,7 +35657,7 @@
         <v>129</v>
       </c>
       <c r="AA339" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AB339" t="s">
         <v>116</v>
@@ -35823,7 +35823,7 @@
         <v>89</v>
       </c>
       <c r="U341" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="V341" t="s">
         <v>87</v>
@@ -35978,7 +35978,7 @@
         <v>85</v>
       </c>
       <c r="I342" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="J342" t="s">
         <v>83</v>
@@ -36008,7 +36008,7 @@
         <v>92</v>
       </c>
       <c r="S342" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="T342" t="s">
         <v>89</v>
@@ -36094,7 +36094,7 @@
         <v>92</v>
       </c>
       <c r="O343" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="P343" t="s">
         <v>89</v>
@@ -36379,7 +36379,7 @@
         <v>121</v>
       </c>
       <c r="J346" t="s">
-        <v>87</v>
+        <v>122</v>
       </c>
       <c r="K346" t="s">
         <v>101</v>
@@ -36418,7 +36418,7 @@
         <v>89</v>
       </c>
       <c r="W346" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="X346" t="s">
         <v>87</v>
@@ -36513,7 +36513,7 @@
         <v>89</v>
       </c>
       <c r="M347" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="N347" t="s">
         <v>87</v>
@@ -36605,7 +36605,7 @@
         <v>89</v>
       </c>
       <c r="W348" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="X348" t="s">
         <v>87</v>
@@ -36778,7 +36778,7 @@
         <v>89</v>
       </c>
       <c r="Y349" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="Z349" t="s">
         <v>87</v>
@@ -36918,7 +36918,7 @@
         <v>89</v>
       </c>
       <c r="W350" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="X350" t="s">
         <v>87</v>
@@ -37090,7 +37090,7 @@
         <v>87</v>
       </c>
       <c r="S352" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="T352" t="s">
         <v>87</v>
@@ -37182,7 +37182,7 @@
         <v>117</v>
       </c>
       <c r="K353" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="L353" t="s">
         <v>89</v>
@@ -37226,10 +37226,10 @@
         <v>85</v>
       </c>
       <c r="I354" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="J354" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="K354" t="s">
         <v>133</v>
@@ -37292,7 +37292,7 @@
         <v>129</v>
       </c>
       <c r="AE354" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="AF354" t="s">
         <v>87</v>
@@ -37516,7 +37516,7 @@
         <v>110</v>
       </c>
       <c r="Q355" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="R355" t="s">
         <v>110</v>
@@ -37642,7 +37642,7 @@
         <v>102</v>
       </c>
       <c r="K358" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="L358" t="s">
         <v>97</v>
@@ -37654,7 +37654,7 @@
         <v>102</v>
       </c>
       <c r="O358" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="P358" t="s">
         <v>97</v>
@@ -37704,7 +37704,7 @@
         <v>102</v>
       </c>
       <c r="K359" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="L359" t="s">
         <v>97</v>
@@ -37716,7 +37716,7 @@
         <v>102</v>
       </c>
       <c r="O359" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="P359" t="s">
         <v>97</v>
@@ -37766,7 +37766,7 @@
         <v>102</v>
       </c>
       <c r="K360" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="L360" t="s">
         <v>97</v>
@@ -37778,7 +37778,7 @@
         <v>102</v>
       </c>
       <c r="O360" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="P360" t="s">
         <v>97</v>
@@ -37828,7 +37828,7 @@
         <v>102</v>
       </c>
       <c r="K361" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="L361" t="s">
         <v>97</v>
@@ -37840,7 +37840,7 @@
         <v>102</v>
       </c>
       <c r="O361" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="P361" t="s">
         <v>97</v>
@@ -37970,10 +37970,10 @@
         <v>122</v>
       </c>
       <c r="K363" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="L363" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="M363" t="s">
         <v>199</v>
@@ -38102,7 +38102,7 @@
         <v>87</v>
       </c>
       <c r="BC363" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="BD363" t="s">
         <v>129</v>
@@ -38259,7 +38259,7 @@
         <v>84</v>
       </c>
       <c r="U365" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="V365" t="s">
         <v>87</v>
@@ -38601,7 +38601,7 @@
         <v>122</v>
       </c>
       <c r="M368" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="N368" t="s">
         <v>122</v>
@@ -38901,13 +38901,13 @@
         <v>106</v>
       </c>
       <c r="K371" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="L371" t="s">
         <v>87</v>
       </c>
       <c r="M371" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="N371" t="s">
         <v>89</v>
@@ -39926,13 +39926,37 @@
     </row>
     <row r="381" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B381" t="s">
         <v>106</v>
       </c>
       <c r="C381" t="s">
         <v>97</v>
+      </c>
+      <c r="I381" t="s">
+        <v>166</v>
+      </c>
+      <c r="J381" t="s">
+        <v>83</v>
+      </c>
+      <c r="K381" t="s">
+        <v>160</v>
+      </c>
+      <c r="L381" t="s">
+        <v>89</v>
+      </c>
+      <c r="M381" t="s">
+        <v>228</v>
+      </c>
+      <c r="N381" t="s">
+        <v>102</v>
+      </c>
+      <c r="O381" t="s">
+        <v>200</v>
+      </c>
+      <c r="P381" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="382" spans="1:66" x14ac:dyDescent="0.35">
@@ -40254,7 +40278,7 @@
         <v>87</v>
       </c>
       <c r="K386" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="L386" t="s">
         <v>100</v>
@@ -40804,31 +40828,31 @@
         <v>85</v>
       </c>
       <c r="I391" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="J391" t="s">
         <v>116</v>
       </c>
       <c r="K391" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="L391" t="s">
         <v>83</v>
       </c>
       <c r="M391" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="N391" t="s">
         <v>116</v>
       </c>
       <c r="O391" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="P391" t="s">
         <v>106</v>
       </c>
       <c r="Q391" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="R391" t="s">
         <v>83</v>
@@ -40878,13 +40902,91 @@
     </row>
     <row r="392" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B392" t="s">
         <v>117</v>
       </c>
       <c r="C392" t="s">
         <v>97</v>
+      </c>
+      <c r="I392" t="s">
+        <v>99</v>
+      </c>
+      <c r="J392" t="s">
+        <v>100</v>
+      </c>
+      <c r="K392" t="s">
+        <v>297</v>
+      </c>
+      <c r="L392" t="s">
+        <v>127</v>
+      </c>
+      <c r="M392" t="s">
+        <v>166</v>
+      </c>
+      <c r="N392" t="s">
+        <v>83</v>
+      </c>
+      <c r="O392" t="s">
+        <v>88</v>
+      </c>
+      <c r="P392" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q392" t="s">
+        <v>90</v>
+      </c>
+      <c r="R392" t="s">
+        <v>89</v>
+      </c>
+      <c r="S392" t="s">
+        <v>168</v>
+      </c>
+      <c r="T392" t="s">
+        <v>108</v>
+      </c>
+      <c r="U392" t="s">
+        <v>137</v>
+      </c>
+      <c r="V392" t="s">
+        <v>102</v>
+      </c>
+      <c r="W392" t="s">
+        <v>177</v>
+      </c>
+      <c r="X392" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y392" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z392" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA392" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB392" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC392" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD392" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE392" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF392" t="s">
+        <v>119</v>
+      </c>
+      <c r="AG392" t="s">
+        <v>811</v>
+      </c>
+      <c r="AH392" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="393" spans="1:90" x14ac:dyDescent="0.35">
@@ -40949,7 +41051,7 @@
         <v>117</v>
       </c>
       <c r="Y393" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="Z393" t="s">
         <v>117</v>
@@ -41032,7 +41134,7 @@
         <v>89</v>
       </c>
       <c r="AC394" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="AD394" t="s">
         <v>87</v>
@@ -41232,7 +41334,7 @@
         <v>85</v>
       </c>
       <c r="I395" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="J395" t="s">
         <v>117</v>
@@ -41408,7 +41510,7 @@
         <v>97</v>
       </c>
       <c r="AM396" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="AN396" t="s">
         <v>129</v>
@@ -41444,7 +41546,7 @@
         <v>84</v>
       </c>
       <c r="AY396" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AZ396" t="s">
         <v>129</v>
@@ -41789,7 +41891,7 @@
         <v>89</v>
       </c>
       <c r="AI399" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="AJ399" t="s">
         <v>87</v>
@@ -41977,7 +42079,7 @@
         <v>117</v>
       </c>
       <c r="M400" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="N400" t="s">
         <v>117</v>
@@ -43074,7 +43176,7 @@
         <v>87</v>
       </c>
       <c r="Q413" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="R413" t="s">
         <v>83</v>
@@ -43086,7 +43188,7 @@
         <v>89</v>
       </c>
       <c r="U413" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="V413" t="s">
         <v>87</v>
@@ -43487,7 +43589,7 @@
         <v>87</v>
       </c>
       <c r="Y417" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="Z417" t="s">
         <v>87</v>
@@ -43945,7 +44047,7 @@
         <v>95</v>
       </c>
       <c r="U424" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="V424" t="s">
         <v>89</v>
@@ -44797,7 +44899,7 @@
         <v>87</v>
       </c>
       <c r="Q433" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="R433" t="s">
         <v>87</v>
@@ -44919,7 +45021,7 @@
         <v>102</v>
       </c>
       <c r="K434" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="L434" t="s">
         <v>84</v>
@@ -45177,7 +45279,7 @@
         <v>119</v>
       </c>
       <c r="U437" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="V437" t="s">
         <v>117</v>
@@ -45415,7 +45517,7 @@
         <v>87</v>
       </c>
       <c r="S439" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="T439" t="s">
         <v>87</v>
@@ -45835,7 +45937,7 @@
         <v>102</v>
       </c>
       <c r="AY442" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="AZ442" t="s">
         <v>92</v>
@@ -45897,7 +45999,7 @@
         <v>117</v>
       </c>
       <c r="S443" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="T443" t="s">
         <v>110</v>
@@ -45995,7 +46097,7 @@
         <v>102</v>
       </c>
       <c r="AC444" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="AD444" t="s">
         <v>110</v>
@@ -46063,7 +46165,7 @@
         <v>89</v>
       </c>
       <c r="M445" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="N445" t="s">
         <v>100</v>
@@ -46125,7 +46227,7 @@
         <v>148</v>
       </c>
       <c r="I446" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="J446" t="s">
         <v>87</v>
@@ -47190,7 +47292,7 @@
         <v>106</v>
       </c>
       <c r="Q455" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="R455" t="s">
         <v>92</v>
@@ -47373,7 +47475,7 @@
         <v>83</v>
       </c>
       <c r="U458" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="V458" t="s">
         <v>110</v>
@@ -47467,7 +47569,7 @@
         <v>95</v>
       </c>
       <c r="O460" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="P460" t="s">
         <v>110</v>
@@ -47573,7 +47675,7 @@
         <v>83</v>
       </c>
       <c r="M462" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="N462" t="s">
         <v>116</v>
@@ -48500,7 +48602,7 @@
         <v>95</v>
       </c>
       <c r="U474" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="V474" t="s">
         <v>119</v>
@@ -48616,7 +48718,7 @@
         <v>102</v>
       </c>
       <c r="AM475" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="AN475" t="s">
         <v>110</v>
@@ -48670,7 +48772,7 @@
         <v>117</v>
       </c>
       <c r="BE475" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="BF475" t="s">
         <v>110</v>
@@ -48902,7 +49004,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="481" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="481" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A481" t="s">
         <v>725</v>
       </c>
@@ -48916,7 +49018,7 @@
         <v>85</v>
       </c>
       <c r="I481" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="J481" t="s">
         <v>122</v>
@@ -48958,7 +49060,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="482" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="482" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A482" t="s">
         <v>726</v>
       </c>
@@ -49017,7 +49119,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="483" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="483" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A483" t="s">
         <v>727</v>
       </c>
@@ -49058,13 +49160,13 @@
         <v>92</v>
       </c>
       <c r="Q483" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="R483" t="s">
         <v>87</v>
       </c>
       <c r="S483" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="T483" t="s">
         <v>89</v>
@@ -49142,7 +49244,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="484" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="484" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A484" t="s">
         <v>728</v>
       </c>
@@ -49222,7 +49324,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="485" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="485" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A485" t="s">
         <v>729</v>
       </c>
@@ -49235,8 +49337,62 @@
       <c r="E485" t="s">
         <v>85</v>
       </c>
+      <c r="I485" t="s">
+        <v>133</v>
+      </c>
+      <c r="J485" t="s">
+        <v>87</v>
+      </c>
+      <c r="K485" t="s">
+        <v>166</v>
+      </c>
+      <c r="L485" t="s">
+        <v>83</v>
+      </c>
+      <c r="M485" t="s">
+        <v>110</v>
+      </c>
+      <c r="N485" t="s">
+        <v>110</v>
+      </c>
+      <c r="O485" t="s">
+        <v>137</v>
+      </c>
+      <c r="P485" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q485" t="s">
+        <v>96</v>
+      </c>
+      <c r="R485" t="s">
+        <v>97</v>
+      </c>
+      <c r="S485" t="s">
+        <v>162</v>
+      </c>
+      <c r="T485" t="s">
+        <v>83</v>
+      </c>
+      <c r="U485" t="s">
+        <v>754</v>
+      </c>
+      <c r="V485" t="s">
+        <v>110</v>
+      </c>
+      <c r="W485" t="s">
+        <v>228</v>
+      </c>
+      <c r="X485" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y485" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z485" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="486" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="486" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A486" t="s">
         <v>730</v>
       </c>
@@ -49246,8 +49402,230 @@
       <c r="E486" t="s">
         <v>85</v>
       </c>
+      <c r="I486" t="s">
+        <v>121</v>
+      </c>
+      <c r="J486" t="s">
+        <v>122</v>
+      </c>
+      <c r="K486" t="s">
+        <v>133</v>
+      </c>
+      <c r="L486" t="s">
+        <v>87</v>
+      </c>
+      <c r="M486" t="s">
+        <v>101</v>
+      </c>
+      <c r="N486" t="s">
+        <v>102</v>
+      </c>
+      <c r="O486" t="s">
+        <v>104</v>
+      </c>
+      <c r="P486" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q486" t="s">
+        <v>124</v>
+      </c>
+      <c r="R486" t="s">
+        <v>87</v>
+      </c>
+      <c r="S486" t="s">
+        <v>185</v>
+      </c>
+      <c r="T486" t="s">
+        <v>83</v>
+      </c>
+      <c r="U486" t="s">
+        <v>176</v>
+      </c>
+      <c r="V486" t="s">
+        <v>127</v>
+      </c>
+      <c r="W486" t="s">
+        <v>93</v>
+      </c>
+      <c r="X486" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y486" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z486" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA486" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB486" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC486" t="s">
+        <v>155</v>
+      </c>
+      <c r="AD486" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE486" t="s">
+        <v>159</v>
+      </c>
+      <c r="AF486" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG486" t="s">
+        <v>157</v>
+      </c>
+      <c r="AH486" t="s">
+        <v>129</v>
+      </c>
+      <c r="AI486" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ486" t="s">
+        <v>119</v>
+      </c>
+      <c r="AK486" t="s">
+        <v>235</v>
+      </c>
+      <c r="AL486" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM486" t="s">
+        <v>203</v>
+      </c>
+      <c r="AN486" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO486" t="s">
+        <v>177</v>
+      </c>
+      <c r="AP486" t="s">
+        <v>83</v>
+      </c>
+      <c r="AQ486" t="s">
+        <v>96</v>
+      </c>
+      <c r="AR486" t="s">
+        <v>97</v>
+      </c>
+      <c r="AS486" t="s">
+        <v>186</v>
+      </c>
+      <c r="AT486" t="s">
+        <v>102</v>
+      </c>
+      <c r="AU486" t="s">
+        <v>113</v>
+      </c>
+      <c r="AV486" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW486" t="s">
+        <v>114</v>
+      </c>
+      <c r="AX486" t="s">
+        <v>110</v>
+      </c>
+      <c r="AY486" t="s">
+        <v>160</v>
+      </c>
+      <c r="AZ486" t="s">
+        <v>89</v>
+      </c>
+      <c r="BA486" t="s">
+        <v>86</v>
+      </c>
+      <c r="BB486" t="s">
+        <v>87</v>
+      </c>
+      <c r="BC486" t="s">
+        <v>150</v>
+      </c>
+      <c r="BD486" t="s">
+        <v>117</v>
+      </c>
+      <c r="BE486" t="s">
+        <v>162</v>
+      </c>
+      <c r="BF486" t="s">
+        <v>83</v>
+      </c>
+      <c r="BG486" t="s">
+        <v>151</v>
+      </c>
+      <c r="BH486" t="s">
+        <v>84</v>
+      </c>
+      <c r="BI486" t="s">
+        <v>94</v>
+      </c>
+      <c r="BJ486" t="s">
+        <v>95</v>
+      </c>
+      <c r="BK486" t="s">
+        <v>153</v>
+      </c>
+      <c r="BL486" t="s">
+        <v>119</v>
+      </c>
+      <c r="BM486" t="s">
+        <v>111</v>
+      </c>
+      <c r="BN486" t="s">
+        <v>97</v>
+      </c>
+      <c r="BO486" t="s">
+        <v>228</v>
+      </c>
+      <c r="BP486" t="s">
+        <v>102</v>
+      </c>
+      <c r="BQ486" t="s">
+        <v>130</v>
+      </c>
+      <c r="BR486" t="s">
+        <v>102</v>
+      </c>
+      <c r="BS486" t="s">
+        <v>187</v>
+      </c>
+      <c r="BT486" t="s">
+        <v>87</v>
+      </c>
+      <c r="BU486" t="s">
+        <v>188</v>
+      </c>
+      <c r="BV486" t="s">
+        <v>87</v>
+      </c>
+      <c r="BW486" t="s">
+        <v>210</v>
+      </c>
+      <c r="BX486" t="s">
+        <v>95</v>
+      </c>
+      <c r="BY486" t="s">
+        <v>146</v>
+      </c>
+      <c r="BZ486" t="s">
+        <v>102</v>
+      </c>
+      <c r="CA486" t="s">
+        <v>131</v>
+      </c>
+      <c r="CB486" t="s">
+        <v>102</v>
+      </c>
+      <c r="CC486" t="s">
+        <v>752</v>
+      </c>
+      <c r="CD486" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="487" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="487" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A487" t="s">
         <v>731</v>
       </c>
@@ -49260,8 +49638,80 @@
       <c r="E487" t="s">
         <v>85</v>
       </c>
+      <c r="I487" t="s">
+        <v>104</v>
+      </c>
+      <c r="J487" t="s">
+        <v>87</v>
+      </c>
+      <c r="K487" t="s">
+        <v>93</v>
+      </c>
+      <c r="L487" t="s">
+        <v>87</v>
+      </c>
+      <c r="M487" t="s">
+        <v>737</v>
+      </c>
+      <c r="N487" t="s">
+        <v>87</v>
+      </c>
+      <c r="O487" t="s">
+        <v>91</v>
+      </c>
+      <c r="P487" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q487" t="s">
+        <v>160</v>
+      </c>
+      <c r="R487" t="s">
+        <v>89</v>
+      </c>
+      <c r="S487" t="s">
+        <v>94</v>
+      </c>
+      <c r="T487" t="s">
+        <v>95</v>
+      </c>
+      <c r="U487" t="s">
+        <v>196</v>
+      </c>
+      <c r="V487" t="s">
+        <v>89</v>
+      </c>
+      <c r="W487" t="s">
+        <v>179</v>
+      </c>
+      <c r="X487" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y487" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z487" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA487" t="s">
+        <v>188</v>
+      </c>
+      <c r="AB487" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC487" t="s">
+        <v>210</v>
+      </c>
+      <c r="AD487" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE487" t="s">
+        <v>174</v>
+      </c>
+      <c r="AF487" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="488" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="488" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A488" t="s">
         <v>732</v>
       </c>
@@ -49271,31 +49721,176 @@
       <c r="E488" t="s">
         <v>85</v>
       </c>
+      <c r="I488" t="s">
+        <v>348</v>
+      </c>
+      <c r="J488" t="s">
+        <v>117</v>
+      </c>
+      <c r="K488" t="s">
+        <v>93</v>
+      </c>
+      <c r="L488" t="s">
+        <v>87</v>
+      </c>
+      <c r="M488" t="s">
+        <v>755</v>
+      </c>
+      <c r="N488" t="s">
+        <v>89</v>
+      </c>
+      <c r="O488" t="s">
+        <v>115</v>
+      </c>
+      <c r="P488" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q488" t="s">
+        <v>194</v>
+      </c>
+      <c r="R488" t="s">
+        <v>106</v>
+      </c>
+      <c r="S488" t="s">
+        <v>217</v>
+      </c>
+      <c r="T488" t="s">
+        <v>92</v>
+      </c>
+      <c r="U488" t="s">
+        <v>145</v>
+      </c>
+      <c r="V488" t="s">
+        <v>89</v>
+      </c>
+      <c r="W488" t="s">
+        <v>131</v>
+      </c>
+      <c r="X488" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="489" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="489" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A489" t="s">
         <v>733</v>
       </c>
       <c r="B489" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="E489" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="490" spans="1:44" x14ac:dyDescent="0.35">
-      <c r="A490" t="s">
-        <v>734</v>
-      </c>
-      <c r="B490" t="s">
-        <v>102</v>
-      </c>
-      <c r="E490" t="s">
-        <v>85</v>
+      <c r="I489" t="s">
+        <v>121</v>
+      </c>
+      <c r="J489" t="s">
+        <v>122</v>
+      </c>
+      <c r="K489" t="s">
+        <v>124</v>
+      </c>
+      <c r="L489" t="s">
+        <v>87</v>
+      </c>
+      <c r="M489" t="s">
+        <v>185</v>
+      </c>
+      <c r="N489" t="s">
+        <v>83</v>
+      </c>
+      <c r="O489" t="s">
+        <v>93</v>
+      </c>
+      <c r="P489" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q489" t="s">
+        <v>155</v>
+      </c>
+      <c r="R489" t="s">
+        <v>117</v>
+      </c>
+      <c r="S489" t="s">
+        <v>110</v>
+      </c>
+      <c r="T489" t="s">
+        <v>110</v>
+      </c>
+      <c r="U489" t="s">
+        <v>126</v>
+      </c>
+      <c r="V489" t="s">
+        <v>127</v>
+      </c>
+      <c r="W489" t="s">
+        <v>115</v>
+      </c>
+      <c r="X489" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y489" t="s">
+        <v>239</v>
+      </c>
+      <c r="Z489" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA489" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB489" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC489" t="s">
+        <v>160</v>
+      </c>
+      <c r="AD489" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE489" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF489" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG489" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH489" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI489" t="s">
+        <v>179</v>
+      </c>
+      <c r="AJ489" t="s">
+        <v>106</v>
+      </c>
+      <c r="AK489" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL489" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM489" t="s">
+        <v>289</v>
+      </c>
+      <c r="AN489" t="s">
+        <v>97</v>
+      </c>
+      <c r="AO489" t="s">
+        <v>209</v>
+      </c>
+      <c r="AP489" t="s">
+        <v>106</v>
+      </c>
+      <c r="AQ489" t="s">
+        <v>188</v>
+      </c>
+      <c r="AR489" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="Q1:Q490" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="Q1:Q489" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Found where Counter was Fighting
</commit_message>
<xml_diff>
--- a/Pokemon.xlsx
+++ b/Pokemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijan Badhya\Documents\Pokemon_elite_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937DE982-8CB3-4DEA-BE6C-A588A0243BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE187F20-3817-4B14-9BC4-E6B448C6DED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2536,7 +2536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2545,9 +2545,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2852,8 +2849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CP489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CF1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="CO2" sqref="CO2"/>
+    <sheetView tabSelected="1" topLeftCell="A268" zoomScale="99" workbookViewId="0">
+      <selection activeCell="J280" sqref="J280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3135,10 +3132,10 @@
       <c r="CN1" s="2" t="s">
         <v>797</v>
       </c>
-      <c r="CO1" s="4" t="s">
+      <c r="CO1" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="CP1" s="4" t="s">
+      <c r="CP1" s="2" t="s">
         <v>812</v>
       </c>
     </row>
@@ -5257,7 +5254,7 @@
         <v>145</v>
       </c>
       <c r="AJ22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:56" x14ac:dyDescent="0.35">
@@ -30055,7 +30052,7 @@
         <v>121</v>
       </c>
       <c r="J280" t="s">
-        <v>87</v>
+        <v>122</v>
       </c>
       <c r="K280" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Proper spelling hunter nd mistype hunter
</commit_message>
<xml_diff>
--- a/Pokemon.xlsx
+++ b/Pokemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijan Badhya\Documents\Pokemon_elite_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5377B2E1-F84A-4982-B68D-9260CCA573F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E0084E-730C-419E-8DEF-5563297F359C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15360" uniqueCount="813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15364" uniqueCount="814">
   <si>
     <t>Name</t>
   </si>
@@ -2462,6 +2462,9 @@
   </si>
   <si>
     <t>Type43</t>
+  </si>
+  <si>
+    <t>Thunder</t>
   </si>
 </sst>
 </file>
@@ -2849,8 +2852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CP489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" zoomScale="99" workbookViewId="0">
-      <selection activeCell="H212" sqref="H212"/>
+    <sheetView tabSelected="1" topLeftCell="T4" zoomScale="99" workbookViewId="0">
+      <selection activeCell="AK23" sqref="AK23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5254,7 +5257,7 @@
         <v>145</v>
       </c>
       <c r="AJ22" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:56" x14ac:dyDescent="0.35">
@@ -16037,171 +16040,177 @@
         <v>122</v>
       </c>
       <c r="K144" t="s">
+        <v>315</v>
+      </c>
+      <c r="L144" t="s">
+        <v>173</v>
+      </c>
+      <c r="M144" t="s">
         <v>348</v>
       </c>
-      <c r="L144" t="s">
+      <c r="N144" t="s">
         <v>117</v>
       </c>
-      <c r="M144" t="s">
+      <c r="O144" t="s">
         <v>101</v>
       </c>
-      <c r="N144" t="s">
-        <v>102</v>
-      </c>
-      <c r="O144" t="s">
+      <c r="P144" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q144" t="s">
         <v>124</v>
       </c>
-      <c r="P144" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q144" t="s">
+      <c r="R144" t="s">
+        <v>87</v>
+      </c>
+      <c r="S144" t="s">
         <v>93</v>
       </c>
-      <c r="R144" t="s">
-        <v>87</v>
-      </c>
-      <c r="S144" t="s">
+      <c r="T144" t="s">
+        <v>87</v>
+      </c>
+      <c r="U144" t="s">
         <v>99</v>
       </c>
-      <c r="T144" t="s">
+      <c r="V144" t="s">
         <v>100</v>
       </c>
-      <c r="U144" t="s">
+      <c r="W144" t="s">
         <v>166</v>
       </c>
-      <c r="V144" t="s">
+      <c r="X144" t="s">
         <v>83</v>
       </c>
-      <c r="W144" t="s">
+      <c r="Y144" t="s">
         <v>316</v>
       </c>
-      <c r="X144" t="s">
+      <c r="Z144" t="s">
         <v>110</v>
       </c>
-      <c r="Y144" t="s">
+      <c r="AA144" t="s">
         <v>225</v>
       </c>
-      <c r="Z144" t="s">
+      <c r="AB144" t="s">
         <v>129</v>
       </c>
-      <c r="AA144" t="s">
+      <c r="AC144" t="s">
         <v>88</v>
       </c>
-      <c r="AB144" t="s">
-        <v>89</v>
-      </c>
-      <c r="AC144" t="s">
+      <c r="AD144" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE144" t="s">
         <v>737</v>
       </c>
-      <c r="AD144" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE144" t="s">
+      <c r="AF144" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG144" t="s">
         <v>159</v>
       </c>
-      <c r="AF144" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG144" t="s">
+      <c r="AH144" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI144" t="s">
         <v>155</v>
       </c>
-      <c r="AH144" t="s">
+      <c r="AJ144" t="s">
         <v>117</v>
       </c>
-      <c r="AI144" t="s">
+      <c r="AK144" t="s">
         <v>156</v>
       </c>
-      <c r="AJ144" t="s">
+      <c r="AL144" t="s">
         <v>84</v>
       </c>
-      <c r="AK144" t="s">
+      <c r="AM144" t="s">
         <v>157</v>
       </c>
-      <c r="AL144" t="s">
+      <c r="AN144" t="s">
         <v>129</v>
       </c>
-      <c r="AM144" t="s">
+      <c r="AO144" t="s">
         <v>137</v>
       </c>
-      <c r="AN144" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO144" t="s">
+      <c r="AP144" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ144" t="s">
         <v>239</v>
       </c>
-      <c r="AP144" t="s">
+      <c r="AR144" t="s">
         <v>110</v>
       </c>
-      <c r="AQ144" t="s">
+      <c r="AS144" t="s">
         <v>96</v>
       </c>
-      <c r="AR144" t="s">
+      <c r="AT144" t="s">
         <v>97</v>
       </c>
-      <c r="AS144" t="s">
+      <c r="AU144" t="s">
         <v>86</v>
       </c>
-      <c r="AT144" t="s">
-        <v>87</v>
-      </c>
-      <c r="AU144" t="s">
+      <c r="AV144" t="s">
+        <v>87</v>
+      </c>
+      <c r="AW144" t="s">
         <v>150</v>
       </c>
-      <c r="AV144" t="s">
+      <c r="AX144" t="s">
         <v>117</v>
       </c>
-      <c r="AW144" t="s">
+      <c r="AY144" t="s">
         <v>151</v>
       </c>
-      <c r="AX144" t="s">
+      <c r="AZ144" t="s">
         <v>84</v>
       </c>
-      <c r="AY144" t="s">
+      <c r="BA144" t="s">
         <v>94</v>
       </c>
-      <c r="AZ144" t="s">
+      <c r="BB144" t="s">
         <v>95</v>
       </c>
-      <c r="BA144" t="s">
+      <c r="BC144" t="s">
         <v>153</v>
       </c>
-      <c r="BB144" t="s">
+      <c r="BD144" t="s">
         <v>119</v>
       </c>
-      <c r="BC144" t="s">
+      <c r="BE144" t="s">
         <v>139</v>
       </c>
-      <c r="BD144" t="s">
+      <c r="BF144" t="s">
         <v>117</v>
       </c>
-      <c r="BE144" t="s">
+      <c r="BG144" t="s">
         <v>140</v>
       </c>
-      <c r="BF144" t="s">
+      <c r="BH144" t="s">
         <v>84</v>
       </c>
-      <c r="BG144" t="s">
+      <c r="BI144" t="s">
         <v>143</v>
       </c>
-      <c r="BH144" t="s">
+      <c r="BJ144" t="s">
         <v>119</v>
       </c>
-      <c r="BI144" t="s">
+      <c r="BK144" t="s">
         <v>149</v>
       </c>
-      <c r="BJ144" t="s">
+      <c r="BL144" t="s">
         <v>84</v>
       </c>
-      <c r="BK144" t="s">
+      <c r="BM144" t="s">
         <v>145</v>
       </c>
-      <c r="BL144" t="s">
-        <v>89</v>
-      </c>
-      <c r="BM144" t="s">
+      <c r="BN144" t="s">
+        <v>89</v>
+      </c>
+      <c r="BO144" t="s">
         <v>210</v>
       </c>
-      <c r="BN144" t="s">
+      <c r="BP144" t="s">
         <v>95</v>
       </c>
     </row>
@@ -37108,75 +37117,81 @@
         <v>87</v>
       </c>
       <c r="S352" t="s">
+        <v>813</v>
+      </c>
+      <c r="T352" t="s">
+        <v>119</v>
+      </c>
+      <c r="U352" t="s">
         <v>737</v>
       </c>
-      <c r="T352" t="s">
-        <v>87</v>
-      </c>
-      <c r="U352" t="s">
+      <c r="V352" t="s">
+        <v>87</v>
+      </c>
+      <c r="W352" t="s">
         <v>125</v>
       </c>
-      <c r="V352" t="s">
+      <c r="X352" t="s">
         <v>83</v>
       </c>
-      <c r="W352" t="s">
+      <c r="Y352" t="s">
         <v>236</v>
       </c>
-      <c r="X352" t="s">
+      <c r="Z352" t="s">
         <v>92</v>
       </c>
-      <c r="Y352" t="s">
+      <c r="AA352" t="s">
         <v>96</v>
       </c>
-      <c r="Z352" t="s">
+      <c r="AB352" t="s">
         <v>97</v>
       </c>
-      <c r="AA352" t="s">
+      <c r="AC352" t="s">
         <v>132</v>
       </c>
-      <c r="AB352" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC352" t="s">
+      <c r="AD352" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE352" t="s">
         <v>150</v>
       </c>
-      <c r="AD352" t="s">
+      <c r="AF352" t="s">
         <v>117</v>
       </c>
-      <c r="AE352" t="s">
+      <c r="AG352" t="s">
         <v>151</v>
       </c>
-      <c r="AF352" t="s">
+      <c r="AH352" t="s">
         <v>84</v>
       </c>
-      <c r="AG352" t="s">
+      <c r="AI352" t="s">
         <v>94</v>
       </c>
-      <c r="AH352" t="s">
+      <c r="AJ352" t="s">
         <v>95</v>
       </c>
-      <c r="AI352" t="s">
+      <c r="AK352" t="s">
         <v>194</v>
       </c>
-      <c r="AJ352" t="s">
+      <c r="AL352" t="s">
         <v>106</v>
       </c>
-      <c r="AK352" t="s">
+      <c r="AM352" t="s">
         <v>153</v>
       </c>
-      <c r="AL352" t="s">
+      <c r="AN352" t="s">
         <v>119</v>
       </c>
-      <c r="AM352" t="s">
+      <c r="AO352" t="s">
         <v>130</v>
       </c>
-      <c r="AN352" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO352" t="s">
+      <c r="AP352" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ352" t="s">
         <v>210</v>
       </c>
-      <c r="AP352" t="s">
+      <c r="AR352" t="s">
         <v>95</v>
       </c>
     </row>
@@ -49914,7 +49929,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="Q1:Q489" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
exploring ways to map dictionary
</commit_message>
<xml_diff>
--- a/Pokemon.xlsx
+++ b/Pokemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijan Badhya\Documents\Pokemon_elite_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E0084E-730C-419E-8DEF-5563297F359C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC79387-F72E-4925-8D1B-3C0D3BAA7C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15364" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15364" uniqueCount="815">
   <si>
     <t>Name</t>
   </si>
@@ -2465,6 +2465,9 @@
   </si>
   <si>
     <t>Thunder</t>
+  </si>
+  <si>
+    <t>Move39</t>
   </si>
 </sst>
 </file>
@@ -2852,8 +2855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CP489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T4" zoomScale="99" workbookViewId="0">
-      <selection activeCell="AK23" sqref="AK23"/>
+    <sheetView tabSelected="1" topLeftCell="BT1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="CH2" sqref="CH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3112,7 +3115,7 @@
         <v>791</v>
       </c>
       <c r="CG1" s="2" t="s">
-        <v>790</v>
+        <v>814</v>
       </c>
       <c r="CH1" s="2" t="s">
         <v>789</v>

</xml_diff>

<commit_message>
Losing my mind planning this
</commit_message>
<xml_diff>
--- a/Pokemon.xlsx
+++ b/Pokemon.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijan Badhya\Documents\Pokemon_elite_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC79387-F72E-4925-8D1B-3C0D3BAA7C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9065821D-DCB6-48E1-B5B1-8C2A2E6DBB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15364" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15356" uniqueCount="815">
   <si>
     <t>Name</t>
   </si>
@@ -2855,8 +2855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CP489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BT1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="CH2" sqref="CH2"/>
+    <sheetView tabSelected="1" topLeftCell="A426" zoomScale="99" workbookViewId="0">
+      <selection activeCell="U437" sqref="U437"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16217,7 +16217,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="145" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>396</v>
       </c>
@@ -16318,7 +16318,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="146" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>397</v>
       </c>
@@ -16416,7 +16416,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="147" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>398</v>
       </c>
@@ -16532,7 +16532,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="148" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>399</v>
       </c>
@@ -16582,7 +16582,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="149" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>400</v>
       </c>
@@ -16749,7 +16749,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="150" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>401</v>
       </c>
@@ -16847,7 +16847,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="151" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>402</v>
       </c>
@@ -16897,7 +16897,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="152" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>403</v>
       </c>
@@ -16953,7 +16953,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="153" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>758</v>
       </c>
@@ -17018,7 +17018,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="154" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>404</v>
       </c>
@@ -17119,7 +17119,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="155" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>405</v>
       </c>
@@ -17196,7 +17196,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="156" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>406</v>
       </c>
@@ -17225,157 +17225,151 @@
         <v>83</v>
       </c>
       <c r="M156" t="s">
-        <v>761</v>
+        <v>88</v>
       </c>
       <c r="N156" t="s">
+        <v>89</v>
+      </c>
+      <c r="O156" t="s">
+        <v>91</v>
+      </c>
+      <c r="P156" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q156" t="s">
+        <v>112</v>
+      </c>
+      <c r="R156" t="s">
+        <v>95</v>
+      </c>
+      <c r="S156" t="s">
+        <v>219</v>
+      </c>
+      <c r="T156" t="s">
         <v>117</v>
       </c>
-      <c r="O156" t="s">
-        <v>88</v>
-      </c>
-      <c r="P156" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q156" t="s">
-        <v>91</v>
-      </c>
-      <c r="R156" t="s">
-        <v>92</v>
-      </c>
-      <c r="S156" t="s">
-        <v>112</v>
-      </c>
-      <c r="T156" t="s">
-        <v>95</v>
-      </c>
       <c r="U156" t="s">
-        <v>219</v>
+        <v>748</v>
       </c>
       <c r="V156" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="W156" t="s">
-        <v>748</v>
+        <v>756</v>
       </c>
       <c r="X156" t="s">
         <v>106</v>
       </c>
       <c r="Y156" t="s">
-        <v>756</v>
+        <v>155</v>
       </c>
       <c r="Z156" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA156" t="s">
+        <v>747</v>
+      </c>
+      <c r="AB156" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC156" t="s">
+        <v>168</v>
+      </c>
+      <c r="AD156" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE156" t="s">
+        <v>137</v>
+      </c>
+      <c r="AF156" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG156" t="s">
+        <v>186</v>
+      </c>
+      <c r="AH156" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI156" t="s">
+        <v>329</v>
+      </c>
+      <c r="AJ156" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK156" t="s">
+        <v>150</v>
+      </c>
+      <c r="AL156" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM156" t="s">
+        <v>162</v>
+      </c>
+      <c r="AN156" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO156" t="s">
+        <v>754</v>
+      </c>
+      <c r="AP156" t="s">
+        <v>110</v>
+      </c>
+      <c r="AQ156" t="s">
+        <v>94</v>
+      </c>
+      <c r="AR156" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS156" t="s">
+        <v>194</v>
+      </c>
+      <c r="AT156" t="s">
         <v>106</v>
       </c>
-      <c r="AA156" t="s">
-        <v>155</v>
-      </c>
-      <c r="AB156" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC156" t="s">
-        <v>747</v>
-      </c>
-      <c r="AD156" t="s">
+      <c r="AU156" t="s">
+        <v>153</v>
+      </c>
+      <c r="AV156" t="s">
+        <v>119</v>
+      </c>
+      <c r="AW156" t="s">
+        <v>170</v>
+      </c>
+      <c r="AX156" t="s">
+        <v>92</v>
+      </c>
+      <c r="AY156" t="s">
+        <v>179</v>
+      </c>
+      <c r="AZ156" t="s">
+        <v>106</v>
+      </c>
+      <c r="BA156" t="s">
+        <v>145</v>
+      </c>
+      <c r="BB156" t="s">
+        <v>89</v>
+      </c>
+      <c r="BC156" t="s">
+        <v>210</v>
+      </c>
+      <c r="BD156" t="s">
+        <v>95</v>
+      </c>
+      <c r="BE156" t="s">
+        <v>308</v>
+      </c>
+      <c r="BF156" t="s">
         <v>116</v>
       </c>
-      <c r="AE156" t="s">
-        <v>168</v>
-      </c>
-      <c r="AF156" t="s">
-        <v>108</v>
-      </c>
-      <c r="AG156" t="s">
-        <v>137</v>
-      </c>
-      <c r="AH156" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI156" t="s">
-        <v>186</v>
-      </c>
-      <c r="AJ156" t="s">
-        <v>102</v>
-      </c>
-      <c r="AK156" t="s">
-        <v>329</v>
-      </c>
-      <c r="AL156" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM156" t="s">
-        <v>150</v>
-      </c>
-      <c r="AN156" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO156" t="s">
-        <v>162</v>
-      </c>
-      <c r="AP156" t="s">
-        <v>83</v>
-      </c>
-      <c r="AQ156" t="s">
-        <v>754</v>
-      </c>
-      <c r="AR156" t="s">
-        <v>110</v>
-      </c>
-      <c r="AS156" t="s">
-        <v>94</v>
-      </c>
-      <c r="AT156" t="s">
-        <v>95</v>
-      </c>
-      <c r="AU156" t="s">
-        <v>194</v>
-      </c>
-      <c r="AV156" t="s">
-        <v>106</v>
-      </c>
-      <c r="AW156" t="s">
-        <v>153</v>
-      </c>
-      <c r="AX156" t="s">
-        <v>119</v>
-      </c>
-      <c r="AY156" t="s">
-        <v>170</v>
-      </c>
-      <c r="AZ156" t="s">
-        <v>92</v>
-      </c>
-      <c r="BA156" t="s">
-        <v>179</v>
-      </c>
-      <c r="BB156" t="s">
-        <v>106</v>
-      </c>
-      <c r="BC156" t="s">
-        <v>145</v>
-      </c>
-      <c r="BD156" t="s">
-        <v>89</v>
-      </c>
-      <c r="BE156" t="s">
-        <v>210</v>
-      </c>
-      <c r="BF156" t="s">
-        <v>95</v>
-      </c>
       <c r="BG156" t="s">
-        <v>308</v>
+        <v>284</v>
       </c>
       <c r="BH156" t="s">
-        <v>116</v>
-      </c>
-      <c r="BI156" t="s">
-        <v>284</v>
-      </c>
-      <c r="BJ156" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="157" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>407</v>
       </c>
@@ -17509,7 +17503,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="158" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>408</v>
       </c>
@@ -17571,7 +17565,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="159" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>409</v>
       </c>
@@ -17633,7 +17627,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="160" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>410</v>
       </c>
@@ -23092,69 +23086,63 @@
         <v>100</v>
       </c>
       <c r="O208" t="s">
-        <v>761</v>
+        <v>225</v>
       </c>
       <c r="P208" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q208" t="s">
+        <v>90</v>
+      </c>
+      <c r="R208" t="s">
+        <v>89</v>
+      </c>
+      <c r="S208" t="s">
+        <v>155</v>
+      </c>
+      <c r="T208" t="s">
         <v>117</v>
       </c>
-      <c r="Q208" t="s">
-        <v>225</v>
-      </c>
-      <c r="R208" t="s">
-        <v>129</v>
-      </c>
-      <c r="S208" t="s">
-        <v>90</v>
-      </c>
-      <c r="T208" t="s">
-        <v>89</v>
-      </c>
       <c r="U208" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="V208" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="W208" t="s">
-        <v>144</v>
+        <v>236</v>
       </c>
       <c r="X208" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="Y208" t="s">
-        <v>236</v>
+        <v>141</v>
       </c>
       <c r="Z208" t="s">
         <v>92</v>
       </c>
       <c r="AA208" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="AB208" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="AC208" t="s">
-        <v>114</v>
+        <v>179</v>
       </c>
       <c r="AD208" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="AE208" t="s">
-        <v>179</v>
+        <v>139</v>
       </c>
       <c r="AF208" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="AG208" t="s">
-        <v>139</v>
+        <v>210</v>
       </c>
       <c r="AH208" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI208" t="s">
-        <v>210</v>
-      </c>
-      <c r="AJ208" t="s">
         <v>95</v>
       </c>
     </row>
@@ -30436,141 +30424,135 @@
         <v>119</v>
       </c>
       <c r="O283" t="s">
-        <v>761</v>
+        <v>159</v>
       </c>
       <c r="P283" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q283" t="s">
+        <v>169</v>
+      </c>
+      <c r="R283" t="s">
+        <v>108</v>
+      </c>
+      <c r="S283" t="s">
+        <v>155</v>
+      </c>
+      <c r="T283" t="s">
         <v>117</v>
       </c>
-      <c r="Q283" t="s">
-        <v>159</v>
-      </c>
-      <c r="R283" t="s">
-        <v>87</v>
-      </c>
-      <c r="S283" t="s">
-        <v>169</v>
-      </c>
-      <c r="T283" t="s">
-        <v>108</v>
-      </c>
       <c r="U283" t="s">
-        <v>155</v>
+        <v>118</v>
       </c>
       <c r="V283" t="s">
+        <v>119</v>
+      </c>
+      <c r="W283" t="s">
+        <v>154</v>
+      </c>
+      <c r="X283" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y283" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z283" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA283" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB283" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC283" t="s">
+        <v>160</v>
+      </c>
+      <c r="AD283" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE283" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF283" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG283" t="s">
+        <v>132</v>
+      </c>
+      <c r="AH283" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI283" t="s">
+        <v>150</v>
+      </c>
+      <c r="AJ283" t="s">
         <v>117</v>
       </c>
-      <c r="W283" t="s">
-        <v>118</v>
-      </c>
-      <c r="X283" t="s">
+      <c r="AK283" t="s">
+        <v>162</v>
+      </c>
+      <c r="AL283" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM283" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN283" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO283" t="s">
+        <v>220</v>
+      </c>
+      <c r="AP283" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ283" t="s">
+        <v>94</v>
+      </c>
+      <c r="AR283" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS283" t="s">
+        <v>153</v>
+      </c>
+      <c r="AT283" t="s">
         <v>119</v>
       </c>
-      <c r="Y283" t="s">
-        <v>154</v>
-      </c>
-      <c r="Z283" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA283" t="s">
-        <v>96</v>
-      </c>
-      <c r="AB283" t="s">
+      <c r="AU283" t="s">
+        <v>289</v>
+      </c>
+      <c r="AV283" t="s">
         <v>97</v>
       </c>
-      <c r="AC283" t="s">
-        <v>114</v>
-      </c>
-      <c r="AD283" t="s">
-        <v>110</v>
-      </c>
-      <c r="AE283" t="s">
-        <v>160</v>
-      </c>
-      <c r="AF283" t="s">
-        <v>89</v>
-      </c>
-      <c r="AG283" t="s">
-        <v>86</v>
-      </c>
-      <c r="AH283" t="s">
-        <v>87</v>
-      </c>
-      <c r="AI283" t="s">
-        <v>132</v>
-      </c>
-      <c r="AJ283" t="s">
-        <v>87</v>
-      </c>
-      <c r="AK283" t="s">
-        <v>150</v>
-      </c>
-      <c r="AL283" t="s">
-        <v>117</v>
-      </c>
-      <c r="AM283" t="s">
-        <v>162</v>
-      </c>
-      <c r="AN283" t="s">
-        <v>83</v>
-      </c>
-      <c r="AO283" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP283" t="s">
-        <v>84</v>
-      </c>
-      <c r="AQ283" t="s">
-        <v>220</v>
-      </c>
-      <c r="AR283" t="s">
-        <v>102</v>
-      </c>
-      <c r="AS283" t="s">
-        <v>94</v>
-      </c>
-      <c r="AT283" t="s">
+      <c r="AW283" t="s">
+        <v>130</v>
+      </c>
+      <c r="AX283" t="s">
+        <v>102</v>
+      </c>
+      <c r="AY283" t="s">
+        <v>765</v>
+      </c>
+      <c r="AZ283" t="s">
+        <v>89</v>
+      </c>
+      <c r="BA283" t="s">
+        <v>210</v>
+      </c>
+      <c r="BB283" t="s">
         <v>95</v>
       </c>
-      <c r="AU283" t="s">
-        <v>153</v>
-      </c>
-      <c r="AV283" t="s">
-        <v>119</v>
-      </c>
-      <c r="AW283" t="s">
-        <v>289</v>
-      </c>
-      <c r="AX283" t="s">
-        <v>97</v>
-      </c>
-      <c r="AY283" t="s">
-        <v>130</v>
-      </c>
-      <c r="AZ283" t="s">
-        <v>102</v>
-      </c>
-      <c r="BA283" t="s">
-        <v>765</v>
-      </c>
-      <c r="BB283" t="s">
-        <v>89</v>
-      </c>
       <c r="BC283" t="s">
-        <v>210</v>
+        <v>146</v>
       </c>
       <c r="BD283" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="BE283" t="s">
-        <v>146</v>
+        <v>227</v>
       </c>
       <c r="BF283" t="s">
-        <v>102</v>
-      </c>
-      <c r="BG283" t="s">
-        <v>227</v>
-      </c>
-      <c r="BH283" t="s">
         <v>97</v>
       </c>
     </row>
@@ -45321,99 +45303,93 @@
         <v>119</v>
       </c>
       <c r="U437" t="s">
-        <v>761</v>
+        <v>219</v>
       </c>
       <c r="V437" t="s">
         <v>117</v>
       </c>
       <c r="W437" t="s">
-        <v>219</v>
+        <v>155</v>
       </c>
       <c r="X437" t="s">
         <v>117</v>
       </c>
       <c r="Y437" t="s">
-        <v>155</v>
+        <v>110</v>
       </c>
       <c r="Z437" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="AA437" t="s">
+        <v>235</v>
+      </c>
+      <c r="AB437" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC437" t="s">
+        <v>239</v>
+      </c>
+      <c r="AD437" t="s">
         <v>110</v>
       </c>
-      <c r="AB437" t="s">
-        <v>110</v>
-      </c>
-      <c r="AC437" t="s">
-        <v>235</v>
-      </c>
-      <c r="AD437" t="s">
-        <v>87</v>
-      </c>
       <c r="AE437" t="s">
-        <v>239</v>
+        <v>164</v>
       </c>
       <c r="AF437" t="s">
         <v>110</v>
       </c>
       <c r="AG437" t="s">
-        <v>164</v>
+        <v>96</v>
       </c>
       <c r="AH437" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI437" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ437" t="s">
         <v>110</v>
       </c>
-      <c r="AI437" t="s">
-        <v>96</v>
-      </c>
-      <c r="AJ437" t="s">
-        <v>97</v>
-      </c>
       <c r="AK437" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="AL437" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="AM437" t="s">
-        <v>86</v>
+        <v>132</v>
       </c>
       <c r="AN437" t="s">
         <v>87</v>
       </c>
       <c r="AO437" t="s">
-        <v>132</v>
+        <v>194</v>
       </c>
       <c r="AP437" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="AQ437" t="s">
-        <v>194</v>
+        <v>163</v>
       </c>
       <c r="AR437" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="AS437" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="AT437" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="AU437" t="s">
-        <v>170</v>
+        <v>217</v>
       </c>
       <c r="AV437" t="s">
         <v>92</v>
       </c>
       <c r="AW437" t="s">
-        <v>217</v>
+        <v>165</v>
       </c>
       <c r="AX437" t="s">
-        <v>92</v>
-      </c>
-      <c r="AY437" t="s">
-        <v>165</v>
-      </c>
-      <c r="AZ437" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Boilerplate of sorting the moves
</commit_message>
<xml_diff>
--- a/Pokemon.xlsx
+++ b/Pokemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijan Badhya\Documents\Pokemon_elite_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9065821D-DCB6-48E1-B5B1-8C2A2E6DBB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0E3A68-09B3-4E61-B769-B6BC978D285B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15356" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15354" uniqueCount="814">
   <si>
     <t>Name</t>
   </si>
@@ -2306,9 +2306,6 @@
   </si>
   <si>
     <t>Petal Blizzard</t>
-  </si>
-  <si>
-    <t>Fire Blast</t>
   </si>
   <si>
     <t>Aqua Cutter</t>
@@ -2855,8 +2852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CP489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A426" zoomScale="99" workbookViewId="0">
-      <selection activeCell="U437" sqref="U437"/>
+    <sheetView tabSelected="1" topLeftCell="L327" zoomScale="99" workbookViewId="0">
+      <selection activeCell="Q334" sqref="Q334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3109,40 +3106,40 @@
         <v>81</v>
       </c>
       <c r="CE1" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="CF1" s="2" t="s">
         <v>790</v>
       </c>
-      <c r="CF1" s="2" t="s">
+      <c r="CG1" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="CH1" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="CI1" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="CJ1" s="2" t="s">
         <v>791</v>
       </c>
-      <c r="CG1" s="2" t="s">
-        <v>814</v>
-      </c>
-      <c r="CH1" s="2" t="s">
-        <v>789</v>
-      </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CK1" s="2" t="s">
         <v>793</v>
       </c>
-      <c r="CJ1" s="2" t="s">
-        <v>792</v>
-      </c>
-      <c r="CK1" s="2" t="s">
+      <c r="CL1" s="2" t="s">
         <v>794</v>
       </c>
-      <c r="CL1" s="2" t="s">
+      <c r="CM1" s="2" t="s">
         <v>795</v>
       </c>
-      <c r="CM1" s="2" t="s">
+      <c r="CN1" s="2" t="s">
         <v>796</v>
       </c>
-      <c r="CN1" s="2" t="s">
-        <v>797</v>
-      </c>
       <c r="CO1" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="CP1" s="2" t="s">
         <v>811</v>
-      </c>
-      <c r="CP1" s="2" t="s">
-        <v>812</v>
       </c>
     </row>
     <row r="2" spans="1:94" x14ac:dyDescent="0.35">
@@ -4069,7 +4066,7 @@
     </row>
     <row r="10" spans="1:94" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B10" t="s">
         <v>83</v>
@@ -4527,7 +4524,7 @@
         <v>102</v>
       </c>
       <c r="BI14" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="BJ14" t="s">
         <v>89</v>
@@ -7609,7 +7606,7 @@
         <v>83</v>
       </c>
       <c r="AE49" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="AF49" t="s">
         <v>89</v>
@@ -12016,7 +12013,7 @@
         <v>102</v>
       </c>
       <c r="AK103" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="AL103" t="s">
         <v>89</v>
@@ -17999,7 +17996,7 @@
         <v>106</v>
       </c>
       <c r="AY162" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="AZ162" t="s">
         <v>129</v>
@@ -18397,7 +18394,7 @@
         <v>106</v>
       </c>
       <c r="AA166" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="AB166" t="s">
         <v>127</v>
@@ -18559,7 +18556,7 @@
     </row>
     <row r="169" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B169" t="s">
         <v>84</v>
@@ -18979,7 +18976,7 @@
         <v>87</v>
       </c>
       <c r="BE172" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="BF172" t="s">
         <v>89</v>
@@ -19113,7 +19110,7 @@
         <v>102</v>
       </c>
       <c r="AQ173" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="AR173" t="s">
         <v>106</v>
@@ -19217,7 +19214,7 @@
         <v>117</v>
       </c>
       <c r="AK174" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="AL174" t="s">
         <v>106</v>
@@ -20339,7 +20336,7 @@
         <v>129</v>
       </c>
       <c r="AG183" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="AH183" t="s">
         <v>129</v>
@@ -21084,7 +21081,7 @@
         <v>97</v>
       </c>
       <c r="AU188" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="AV188" t="s">
         <v>106</v>
@@ -21119,7 +21116,7 @@
         <v>102</v>
       </c>
       <c r="K189" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="L189" t="s">
         <v>89</v>
@@ -21239,7 +21236,7 @@
         <v>102</v>
       </c>
       <c r="AY189" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="AZ189" t="s">
         <v>92</v>
@@ -21703,7 +21700,7 @@
         <v>95</v>
       </c>
       <c r="AG193" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="AH193" t="s">
         <v>92</v>
@@ -21750,7 +21747,7 @@
         <v>95</v>
       </c>
       <c r="O194" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="P194" t="s">
         <v>117</v>
@@ -21810,7 +21807,7 @@
         <v>95</v>
       </c>
       <c r="AI194" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="AJ194" t="s">
         <v>92</v>
@@ -21899,7 +21896,7 @@
         <v>116</v>
       </c>
       <c r="AC195" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="AD195" t="s">
         <v>102</v>
@@ -21917,7 +21914,7 @@
         <v>102</v>
       </c>
       <c r="AI195" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="AJ195" t="s">
         <v>92</v>
@@ -21949,7 +21946,7 @@
         <v>85</v>
       </c>
       <c r="I196" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="J196" t="s">
         <v>122</v>
@@ -22157,7 +22154,7 @@
         <v>122</v>
       </c>
       <c r="K198" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="L198" t="s">
         <v>122</v>
@@ -24312,7 +24309,7 @@
     </row>
     <row r="221" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B221" t="s">
         <v>106</v>
@@ -24549,7 +24546,7 @@
         <v>87</v>
       </c>
       <c r="S224" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="T224" t="s">
         <v>83</v>
@@ -25405,7 +25402,7 @@
         <v>110</v>
       </c>
       <c r="AI232" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="AJ232" t="s">
         <v>87</v>
@@ -25856,7 +25853,7 @@
         <v>87</v>
       </c>
       <c r="M237" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="N237" t="s">
         <v>87</v>
@@ -25912,7 +25909,7 @@
         <v>87</v>
       </c>
       <c r="M238" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="N238" t="s">
         <v>87</v>
@@ -25990,7 +25987,7 @@
         <v>116</v>
       </c>
       <c r="AM238" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="AN238" t="s">
         <v>87</v>
@@ -26106,7 +26103,7 @@
         <v>110</v>
       </c>
       <c r="Q239" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="R239" t="s">
         <v>117</v>
@@ -26190,7 +26187,7 @@
         <v>102</v>
       </c>
       <c r="AS239" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="AT239" t="s">
         <v>89</v>
@@ -27086,7 +27083,7 @@
         <v>85</v>
       </c>
       <c r="I249" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="J249" t="s">
         <v>122</v>
@@ -27175,123 +27172,117 @@
         <v>92</v>
       </c>
       <c r="O250" t="s">
-        <v>761</v>
+        <v>88</v>
       </c>
       <c r="P250" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q250" t="s">
+        <v>112</v>
+      </c>
+      <c r="R250" t="s">
+        <v>95</v>
+      </c>
+      <c r="S250" t="s">
+        <v>155</v>
+      </c>
+      <c r="T250" t="s">
         <v>117</v>
       </c>
-      <c r="Q250" t="s">
-        <v>88</v>
-      </c>
-      <c r="R250" t="s">
-        <v>89</v>
-      </c>
-      <c r="S250" t="s">
-        <v>112</v>
-      </c>
-      <c r="T250" t="s">
+      <c r="U250" t="s">
+        <v>273</v>
+      </c>
+      <c r="V250" t="s">
+        <v>102</v>
+      </c>
+      <c r="W250" t="s">
+        <v>203</v>
+      </c>
+      <c r="X250" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y250" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z250" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA250" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB250" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC250" t="s">
+        <v>150</v>
+      </c>
+      <c r="AD250" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE250" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF250" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG250" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH250" t="s">
         <v>95</v>
       </c>
-      <c r="U250" t="s">
-        <v>155</v>
-      </c>
-      <c r="V250" t="s">
-        <v>117</v>
-      </c>
-      <c r="W250" t="s">
-        <v>273</v>
-      </c>
-      <c r="X250" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y250" t="s">
-        <v>203</v>
-      </c>
-      <c r="Z250" t="s">
+      <c r="AI250" t="s">
+        <v>153</v>
+      </c>
+      <c r="AJ250" t="s">
+        <v>119</v>
+      </c>
+      <c r="AK250" t="s">
+        <v>233</v>
+      </c>
+      <c r="AL250" t="s">
         <v>127</v>
       </c>
-      <c r="AA250" t="s">
-        <v>186</v>
-      </c>
-      <c r="AB250" t="s">
-        <v>102</v>
-      </c>
-      <c r="AC250" t="s">
-        <v>160</v>
-      </c>
-      <c r="AD250" t="s">
-        <v>89</v>
-      </c>
-      <c r="AE250" t="s">
-        <v>150</v>
-      </c>
-      <c r="AF250" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG250" t="s">
-        <v>151</v>
-      </c>
-      <c r="AH250" t="s">
-        <v>84</v>
-      </c>
-      <c r="AI250" t="s">
-        <v>94</v>
-      </c>
-      <c r="AJ250" t="s">
+      <c r="AM250" t="s">
+        <v>130</v>
+      </c>
+      <c r="AN250" t="s">
+        <v>102</v>
+      </c>
+      <c r="AO250" t="s">
+        <v>145</v>
+      </c>
+      <c r="AP250" t="s">
+        <v>89</v>
+      </c>
+      <c r="AQ250" t="s">
+        <v>210</v>
+      </c>
+      <c r="AR250" t="s">
         <v>95</v>
       </c>
-      <c r="AK250" t="s">
-        <v>153</v>
-      </c>
-      <c r="AL250" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM250" t="s">
-        <v>233</v>
-      </c>
-      <c r="AN250" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO250" t="s">
-        <v>130</v>
-      </c>
-      <c r="AP250" t="s">
-        <v>102</v>
-      </c>
-      <c r="AQ250" t="s">
-        <v>145</v>
-      </c>
-      <c r="AR250" t="s">
-        <v>89</v>
-      </c>
       <c r="AS250" t="s">
-        <v>210</v>
+        <v>146</v>
       </c>
       <c r="AT250" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="AU250" t="s">
-        <v>146</v>
+        <v>768</v>
       </c>
       <c r="AV250" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="AW250" t="s">
-        <v>769</v>
+        <v>180</v>
       </c>
       <c r="AX250" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="AY250" t="s">
-        <v>180</v>
+        <v>223</v>
       </c>
       <c r="AZ250" t="s">
-        <v>100</v>
-      </c>
-      <c r="BA250" t="s">
-        <v>223</v>
-      </c>
-      <c r="BB250" t="s">
         <v>95</v>
       </c>
     </row>
@@ -27491,7 +27482,7 @@
         <v>95</v>
       </c>
       <c r="BA252" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="BB252" t="s">
         <v>87</v>
@@ -27621,7 +27612,7 @@
         <v>95</v>
       </c>
       <c r="S254" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="T254" t="s">
         <v>89</v>
@@ -27674,7 +27665,7 @@
         <v>106</v>
       </c>
       <c r="U255" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="V255" t="s">
         <v>117</v>
@@ -28114,7 +28105,7 @@
         <v>102</v>
       </c>
       <c r="BC259" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="BD259" t="s">
         <v>89</v>
@@ -28132,13 +28123,13 @@
         <v>95</v>
       </c>
       <c r="BI259" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="BJ259" t="s">
         <v>89</v>
       </c>
       <c r="BK259" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="BL259" t="s">
         <v>89</v>
@@ -28921,7 +28912,7 @@
     </row>
     <row r="268" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B268" t="s">
         <v>110</v>
@@ -29581,7 +29572,7 @@
         <v>102</v>
       </c>
       <c r="K274" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="L274" t="s">
         <v>83</v>
@@ -29806,7 +29797,7 @@
         <v>119</v>
       </c>
       <c r="O277" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="P277" t="s">
         <v>117</v>
@@ -30532,7 +30523,7 @@
         <v>102</v>
       </c>
       <c r="AY283" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="AZ283" t="s">
         <v>89</v>
@@ -30713,7 +30704,7 @@
         <v>83</v>
       </c>
       <c r="O285" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="P285" t="s">
         <v>97</v>
@@ -30766,7 +30757,7 @@
         <v>92</v>
       </c>
       <c r="K286" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="L286" t="s">
         <v>108</v>
@@ -33618,7 +33609,7 @@
     </row>
     <row r="317" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="B317" t="s">
         <v>129</v>
@@ -34444,13 +34435,13 @@
         <v>102</v>
       </c>
       <c r="AI325" t="s">
+        <v>786</v>
+      </c>
+      <c r="AJ325" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK325" t="s">
         <v>787</v>
-      </c>
-      <c r="AJ325" t="s">
-        <v>87</v>
-      </c>
-      <c r="AK325" t="s">
-        <v>788</v>
       </c>
       <c r="AL325" t="s">
         <v>87</v>
@@ -34744,7 +34735,7 @@
         <v>102</v>
       </c>
       <c r="AI328" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="AJ328" t="s">
         <v>89</v>
@@ -35446,7 +35437,7 @@
         <v>127</v>
       </c>
       <c r="M337" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="N337" t="s">
         <v>97</v>
@@ -37102,7 +37093,7 @@
         <v>87</v>
       </c>
       <c r="S352" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="T352" t="s">
         <v>119</v>
@@ -37666,7 +37657,7 @@
         <v>102</v>
       </c>
       <c r="K358" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="L358" t="s">
         <v>97</v>
@@ -37728,7 +37719,7 @@
         <v>102</v>
       </c>
       <c r="K359" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="L359" t="s">
         <v>97</v>
@@ -37790,7 +37781,7 @@
         <v>102</v>
       </c>
       <c r="K360" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="L360" t="s">
         <v>97</v>
@@ -37852,7 +37843,7 @@
         <v>102</v>
       </c>
       <c r="K361" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="L361" t="s">
         <v>97</v>
@@ -38126,7 +38117,7 @@
         <v>87</v>
       </c>
       <c r="BC363" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="BD363" t="s">
         <v>129</v>
@@ -38283,7 +38274,7 @@
         <v>84</v>
       </c>
       <c r="U365" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="V365" t="s">
         <v>87</v>
@@ -39950,7 +39941,7 @@
     </row>
     <row r="381" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B381" t="s">
         <v>106</v>
@@ -40302,7 +40293,7 @@
         <v>87</v>
       </c>
       <c r="K386" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="L386" t="s">
         <v>100</v>
@@ -40926,7 +40917,7 @@
     </row>
     <row r="392" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B392" t="s">
         <v>117</v>
@@ -41007,7 +40998,7 @@
         <v>119</v>
       </c>
       <c r="AG392" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="AH392" t="s">
         <v>102</v>
@@ -41075,7 +41066,7 @@
         <v>117</v>
       </c>
       <c r="Y393" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="Z393" t="s">
         <v>117</v>
@@ -41358,7 +41349,7 @@
         <v>85</v>
       </c>
       <c r="I395" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="J395" t="s">
         <v>117</v>
@@ -42103,7 +42094,7 @@
         <v>117</v>
       </c>
       <c r="M400" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="N400" t="s">
         <v>117</v>
@@ -43200,7 +43191,7 @@
         <v>87</v>
       </c>
       <c r="Q413" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="R413" t="s">
         <v>83</v>
@@ -45045,7 +45036,7 @@
         <v>102</v>
       </c>
       <c r="K434" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="L434" t="s">
         <v>84</v>
@@ -45955,7 +45946,7 @@
         <v>102</v>
       </c>
       <c r="AY442" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="AZ442" t="s">
         <v>92</v>
@@ -46183,7 +46174,7 @@
         <v>89</v>
       </c>
       <c r="M445" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="N445" t="s">
         <v>100</v>
@@ -46245,7 +46236,7 @@
         <v>148</v>
       </c>
       <c r="I446" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="J446" t="s">
         <v>87</v>
@@ -47310,7 +47301,7 @@
         <v>106</v>
       </c>
       <c r="Q455" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="R455" t="s">
         <v>92</v>
@@ -48620,7 +48611,7 @@
         <v>95</v>
       </c>
       <c r="U474" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="V474" t="s">
         <v>119</v>
@@ -48736,7 +48727,7 @@
         <v>102</v>
       </c>
       <c r="AM475" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="AN475" t="s">
         <v>110</v>

</xml_diff>

<commit_message>
SUCCESSFULLY SORTED EVERYTHING BEAUTIFULLY
</commit_message>
<xml_diff>
--- a/Pokemon.xlsx
+++ b/Pokemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijan Badhya\Documents\Pokemon_elite_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0E3A68-09B3-4E61-B769-B6BC978D285B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433E07FC-D036-4C1B-899A-417ACCC398BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15354" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15348" uniqueCount="814">
   <si>
     <t>Name</t>
   </si>
@@ -2852,8 +2852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CP489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L327" zoomScale="99" workbookViewId="0">
-      <selection activeCell="Q334" sqref="Q334"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="AG21" sqref="AG21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4034,33 +4034,27 @@
         <v>119</v>
       </c>
       <c r="BU9" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="BV9" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="BW9" t="s">
-        <v>190</v>
+        <v>115</v>
       </c>
       <c r="BX9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="BY9" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="BZ9" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="CA9" t="s">
-        <v>160</v>
+        <v>191</v>
       </c>
       <c r="CB9" t="s">
-        <v>89</v>
-      </c>
-      <c r="CC9" t="s">
-        <v>191</v>
-      </c>
-      <c r="CD9" t="s">
         <v>102</v>
       </c>
     </row>
@@ -4674,12 +4668,6 @@
       <c r="AL16" t="s">
         <v>89</v>
       </c>
-      <c r="AM16" t="s">
-        <v>215</v>
-      </c>
-      <c r="AN16" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="17" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
@@ -5138,27 +5126,21 @@
         <v>83</v>
       </c>
       <c r="AG21" t="s">
-        <v>196</v>
+        <v>228</v>
       </c>
       <c r="AH21" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="AI21" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AJ21" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="AK21" t="s">
-        <v>229</v>
+        <v>131</v>
       </c>
       <c r="AL21" t="s">
-        <v>110</v>
-      </c>
-      <c r="AM21" t="s">
-        <v>131</v>
-      </c>
-      <c r="AN21" t="s">
         <v>102</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Perfected the Freeze Dry code and included in stab
</commit_message>
<xml_diff>
--- a/Pokemon.xlsx
+++ b/Pokemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijan Badhya\Documents\Pokemon_elite_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4760F2-338C-4568-914F-F434696A6ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618D5864-9134-4FF2-9145-E83762797400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$T$1:$T$489</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$1:$D$489</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15352" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15376" uniqueCount="819">
   <si>
     <t>Name</t>
   </si>
@@ -2867,8 +2867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CS489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="99" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="A277" zoomScale="99" workbookViewId="0">
+      <selection activeCell="D290" sqref="D290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11613,7 +11613,7 @@
         <v>222</v>
       </c>
       <c r="M95" t="s">
-        <v>119</v>
+        <v>222</v>
       </c>
       <c r="N95" t="s">
         <v>236</v>
@@ -12462,7 +12462,7 @@
         <v>222</v>
       </c>
       <c r="M104" t="s">
-        <v>119</v>
+        <v>222</v>
       </c>
       <c r="N104" t="s">
         <v>121</v>
@@ -15337,7 +15337,7 @@
         <v>222</v>
       </c>
       <c r="M130" t="s">
-        <v>119</v>
+        <v>222</v>
       </c>
       <c r="N130" t="s">
         <v>133</v>
@@ -18920,7 +18920,7 @@
         <v>222</v>
       </c>
       <c r="M168" t="s">
-        <v>119</v>
+        <v>222</v>
       </c>
       <c r="N168" t="s">
         <v>204</v>
@@ -25355,7 +25355,7 @@
         <v>222</v>
       </c>
       <c r="M228" t="s">
-        <v>119</v>
+        <v>222</v>
       </c>
       <c r="N228" t="s">
         <v>120</v>
@@ -30615,7 +30615,7 @@
         <v>222</v>
       </c>
       <c r="M281" t="s">
-        <v>119</v>
+        <v>222</v>
       </c>
       <c r="N281" t="s">
         <v>204</v>
@@ -32008,7 +32008,79 @@
         <v>222</v>
       </c>
       <c r="M292" t="s">
-        <v>119</v>
+        <v>222</v>
+      </c>
+      <c r="N292" t="s">
+        <v>166</v>
+      </c>
+      <c r="O292" t="s">
+        <v>83</v>
+      </c>
+      <c r="P292" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q292" t="s">
+        <v>102</v>
+      </c>
+      <c r="R292" t="s">
+        <v>136</v>
+      </c>
+      <c r="S292" t="s">
+        <v>129</v>
+      </c>
+      <c r="T292" t="s">
+        <v>154</v>
+      </c>
+      <c r="U292" t="s">
+        <v>102</v>
+      </c>
+      <c r="V292" t="s">
+        <v>239</v>
+      </c>
+      <c r="W292" t="s">
+        <v>110</v>
+      </c>
+      <c r="X292" t="s">
+        <v>164</v>
+      </c>
+      <c r="Y292" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z292" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA292" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB292" t="s">
+        <v>160</v>
+      </c>
+      <c r="AC292" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD292" t="s">
+        <v>289</v>
+      </c>
+      <c r="AE292" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF292" t="s">
+        <v>146</v>
+      </c>
+      <c r="AG292" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH292" t="s">
+        <v>165</v>
+      </c>
+      <c r="AI292" t="s">
+        <v>110</v>
+      </c>
+      <c r="AJ292" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK292" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="293" spans="1:77" x14ac:dyDescent="0.35">
@@ -50322,6 +50394,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="D1:D489" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Contact categories, pulse, sound based moves added
</commit_message>
<xml_diff>
--- a/Pokemon.xlsx
+++ b/Pokemon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijan Badhya\Documents\Pokemon_elite_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3701B16-4DBD-400E-B64B-F0251E61033F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65D62C7-D4F3-426B-836F-B586B7D7843A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15378" uniqueCount="820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15380" uniqueCount="820">
   <si>
     <t>Name</t>
   </si>
@@ -2254,9 +2254,6 @@
     <t>Jump Kick</t>
   </si>
   <si>
-    <t>Assurance</t>
-  </si>
-  <si>
     <t>Ice Shard</t>
   </si>
   <si>
@@ -2483,6 +2480,9 @@
   </si>
   <si>
     <t>UU</t>
+  </si>
+  <si>
+    <t>Snarl</t>
   </si>
 </sst>
 </file>
@@ -2870,8 +2870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CS489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL210" zoomScale="99" workbookViewId="0">
-      <selection activeCell="AR221" sqref="AR221"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="99" workbookViewId="0">
+      <selection activeCell="M130" sqref="M130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2890,13 +2890,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>815</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>816</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -3133,40 +3133,40 @@
         <v>81</v>
       </c>
       <c r="CH1" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="CI1" s="2" t="s">
         <v>789</v>
       </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CJ1" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="CK1" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="CL1" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="CM1" s="2" t="s">
         <v>790</v>
       </c>
-      <c r="CJ1" s="2" t="s">
-        <v>813</v>
-      </c>
-      <c r="CK1" s="2" t="s">
-        <v>788</v>
-      </c>
-      <c r="CL1" s="2" t="s">
+      <c r="CN1" s="2" t="s">
         <v>792</v>
       </c>
-      <c r="CM1" s="2" t="s">
-        <v>791</v>
-      </c>
-      <c r="CN1" s="2" t="s">
+      <c r="CO1" s="2" t="s">
         <v>793</v>
       </c>
-      <c r="CO1" s="2" t="s">
+      <c r="CP1" s="2" t="s">
         <v>794</v>
       </c>
-      <c r="CP1" s="2" t="s">
+      <c r="CQ1" s="2" t="s">
         <v>795</v>
       </c>
-      <c r="CQ1" s="2" t="s">
-        <v>796</v>
-      </c>
       <c r="CR1" s="2" t="s">
+        <v>809</v>
+      </c>
+      <c r="CS1" s="2" t="s">
         <v>810</v>
-      </c>
-      <c r="CS1" s="2" t="s">
-        <v>811</v>
       </c>
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.35">
@@ -4135,7 +4135,7 @@
     </row>
     <row r="10" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B10" t="s">
         <v>83</v>
@@ -4623,7 +4623,7 @@
         <v>102</v>
       </c>
       <c r="BL14" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="BM14" t="s">
         <v>89</v>
@@ -5065,7 +5065,7 @@
         <v>222</v>
       </c>
       <c r="Y19" t="s">
-        <v>119</v>
+        <v>222</v>
       </c>
       <c r="Z19" t="s">
         <v>210</v>
@@ -5103,7 +5103,7 @@
         <v>222</v>
       </c>
       <c r="M20" t="s">
-        <v>119</v>
+        <v>222</v>
       </c>
       <c r="N20" t="s">
         <v>91</v>
@@ -5566,7 +5566,7 @@
         <v>222</v>
       </c>
       <c r="O25" t="s">
-        <v>119</v>
+        <v>222</v>
       </c>
       <c r="P25" t="s">
         <v>194</v>
@@ -5818,7 +5818,7 @@
         <v>222</v>
       </c>
       <c r="M28" t="s">
-        <v>119</v>
+        <v>222</v>
       </c>
       <c r="N28" t="s">
         <v>154</v>
@@ -5999,7 +5999,7 @@
         <v>34</v>
       </c>
       <c r="G30" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H30" t="s">
         <v>85</v>
@@ -6216,7 +6216,7 @@
         <v>60</v>
       </c>
       <c r="H32" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="L32" t="s">
         <v>86</v>
@@ -6974,7 +6974,7 @@
         <v>89</v>
       </c>
       <c r="AN39" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="AO39" t="s">
         <v>122</v>
@@ -7900,7 +7900,7 @@
         <v>83</v>
       </c>
       <c r="AH49" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="AI49" t="s">
         <v>89</v>
@@ -10615,7 +10615,7 @@
         <v>95</v>
       </c>
       <c r="AB82" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="AC82" t="s">
         <v>122</v>
@@ -12631,7 +12631,7 @@
         <v>102</v>
       </c>
       <c r="AN103" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="AO103" t="s">
         <v>89</v>
@@ -13704,21 +13704,15 @@
         <v>119</v>
       </c>
       <c r="BD113" t="s">
+        <v>210</v>
+      </c>
+      <c r="BE113" t="s">
+        <v>95</v>
+      </c>
+      <c r="BF113" t="s">
         <v>743</v>
       </c>
-      <c r="BE113" t="s">
-        <v>102</v>
-      </c>
-      <c r="BF113" t="s">
-        <v>210</v>
-      </c>
       <c r="BG113" t="s">
-        <v>95</v>
-      </c>
-      <c r="BH113" t="s">
-        <v>744</v>
-      </c>
-      <c r="BI113" t="s">
         <v>84</v>
       </c>
     </row>
@@ -13739,7 +13733,7 @@
         <v>80</v>
       </c>
       <c r="H114" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="L114" t="s">
         <v>93</v>
@@ -13906,7 +13900,7 @@
         <v>129</v>
       </c>
       <c r="AJ115" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="AK115" t="s">
         <v>129</v>
@@ -13918,7 +13912,7 @@
         <v>129</v>
       </c>
       <c r="AN115" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="AO115" t="s">
         <v>129</v>
@@ -14028,7 +14022,7 @@
         <v>119</v>
       </c>
       <c r="AN116" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="AO116" t="s">
         <v>116</v>
@@ -14114,7 +14108,7 @@
         <v>129</v>
       </c>
       <c r="R117" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="S117" t="s">
         <v>106</v>
@@ -14278,7 +14272,7 @@
         <v>89</v>
       </c>
       <c r="AJ118" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="AK118" t="s">
         <v>102</v>
@@ -15162,7 +15156,7 @@
         <v>95</v>
       </c>
       <c r="AJ125" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="AK125" t="s">
         <v>122</v>
@@ -15188,7 +15182,7 @@
         <v>85</v>
       </c>
       <c r="L126" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="M126" t="s">
         <v>122</v>
@@ -15733,7 +15727,7 @@
         <v>92</v>
       </c>
       <c r="Z130" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="AA130" t="s">
         <v>129</v>
@@ -15757,7 +15751,7 @@
         <v>129</v>
       </c>
       <c r="AH130" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="AI130" t="s">
         <v>129</v>
@@ -16281,7 +16275,7 @@
         <v>84</v>
       </c>
       <c r="T137" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="U137" t="s">
         <v>116</v>
@@ -16377,7 +16371,7 @@
         <v>84</v>
       </c>
       <c r="AZ137" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="BA137" t="s">
         <v>102</v>
@@ -16626,7 +16620,7 @@
         <v>83</v>
       </c>
       <c r="AB140" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="AC140" t="s">
         <v>129</v>
@@ -16851,7 +16845,7 @@
         <v>87</v>
       </c>
       <c r="AH143" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AI143" t="s">
         <v>110</v>
@@ -17107,13 +17101,13 @@
         <v>106</v>
       </c>
       <c r="P145" t="s">
+        <v>754</v>
+      </c>
+      <c r="Q145" t="s">
+        <v>89</v>
+      </c>
+      <c r="R145" t="s">
         <v>755</v>
-      </c>
-      <c r="Q145" t="s">
-        <v>89</v>
-      </c>
-      <c r="R145" t="s">
-        <v>756</v>
       </c>
       <c r="S145" t="s">
         <v>106</v>
@@ -17235,13 +17229,13 @@
         <v>117</v>
       </c>
       <c r="V146" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="W146" t="s">
         <v>106</v>
       </c>
       <c r="X146" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="Y146" t="s">
         <v>83</v>
@@ -17678,7 +17672,7 @@
         <v>117</v>
       </c>
       <c r="R150" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="S150" t="s">
         <v>116</v>
@@ -17826,7 +17820,7 @@
         <v>92</v>
       </c>
       <c r="N152" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="O152" t="s">
         <v>116</v>
@@ -17864,7 +17858,7 @@
     </row>
     <row r="153" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B153" t="s">
         <v>117</v>
@@ -18063,7 +18057,7 @@
         <v>83</v>
       </c>
       <c r="N155" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="O155" t="s">
         <v>83</v>
@@ -18081,7 +18075,7 @@
         <v>83</v>
       </c>
       <c r="T155" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="U155" t="s">
         <v>83</v>
@@ -18111,7 +18105,7 @@
         <v>83</v>
       </c>
       <c r="AD155" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AE155" t="s">
         <v>110</v>
@@ -18182,13 +18176,13 @@
         <v>117</v>
       </c>
       <c r="X156" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="Y156" t="s">
         <v>106</v>
       </c>
       <c r="Z156" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="AA156" t="s">
         <v>106</v>
@@ -18200,7 +18194,7 @@
         <v>117</v>
       </c>
       <c r="AD156" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="AE156" t="s">
         <v>116</v>
@@ -18242,7 +18236,7 @@
         <v>83</v>
       </c>
       <c r="AR156" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AS156" t="s">
         <v>110</v>
@@ -18884,7 +18878,7 @@
         <v>119</v>
       </c>
       <c r="Z162" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="AA162" t="s">
         <v>83</v>
@@ -18968,7 +18962,7 @@
         <v>106</v>
       </c>
       <c r="BB162" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="BC162" t="s">
         <v>129</v>
@@ -19396,7 +19390,7 @@
         <v>106</v>
       </c>
       <c r="AD166" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="AE166" t="s">
         <v>127</v>
@@ -19570,7 +19564,7 @@
     </row>
     <row r="169" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B169" t="s">
         <v>84</v>
@@ -19588,7 +19582,7 @@
         <v>222</v>
       </c>
       <c r="M169" t="s">
-        <v>119</v>
+        <v>222</v>
       </c>
       <c r="N169" t="s">
         <v>199</v>
@@ -19984,7 +19978,7 @@
         <v>84</v>
       </c>
       <c r="AX172" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AY172" t="s">
         <v>110</v>
@@ -20014,7 +20008,7 @@
         <v>87</v>
       </c>
       <c r="BH172" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="BI172" t="s">
         <v>89</v>
@@ -20154,7 +20148,7 @@
         <v>102</v>
       </c>
       <c r="AT173" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="AU173" t="s">
         <v>106</v>
@@ -20264,7 +20258,7 @@
         <v>117</v>
       </c>
       <c r="AN174" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="AO174" t="s">
         <v>106</v>
@@ -20532,7 +20526,7 @@
         <v>119</v>
       </c>
       <c r="AT176" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="AU176" t="s">
         <v>116</v>
@@ -21344,7 +21338,7 @@
         <v>129</v>
       </c>
       <c r="T183" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="U183" t="s">
         <v>129</v>
@@ -21392,7 +21386,7 @@
         <v>129</v>
       </c>
       <c r="AJ183" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="AK183" t="s">
         <v>129</v>
@@ -22137,7 +22131,7 @@
         <v>97</v>
       </c>
       <c r="AX188" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="AY188" t="s">
         <v>106</v>
@@ -22172,7 +22166,7 @@
         <v>102</v>
       </c>
       <c r="N189" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="O189" t="s">
         <v>89</v>
@@ -22292,7 +22286,7 @@
         <v>102</v>
       </c>
       <c r="BB189" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="BC189" t="s">
         <v>92</v>
@@ -22756,7 +22750,7 @@
         <v>95</v>
       </c>
       <c r="AJ193" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="AK193" t="s">
         <v>92</v>
@@ -22803,7 +22797,7 @@
         <v>95</v>
       </c>
       <c r="R194" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="S194" t="s">
         <v>117</v>
@@ -22863,7 +22857,7 @@
         <v>95</v>
       </c>
       <c r="AL194" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="AM194" t="s">
         <v>92</v>
@@ -22952,7 +22946,7 @@
         <v>116</v>
       </c>
       <c r="AF195" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="AG195" t="s">
         <v>102</v>
@@ -22970,7 +22964,7 @@
         <v>102</v>
       </c>
       <c r="AL195" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="AM195" t="s">
         <v>92</v>
@@ -23002,7 +22996,7 @@
         <v>85</v>
       </c>
       <c r="L196" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="M196" t="s">
         <v>122</v>
@@ -23032,7 +23026,7 @@
         <v>97</v>
       </c>
       <c r="V196" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="W196" t="s">
         <v>110</v>
@@ -23210,7 +23204,7 @@
         <v>122</v>
       </c>
       <c r="N198" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="O198" t="s">
         <v>122</v>
@@ -24083,7 +24077,7 @@
         <v>116</v>
       </c>
       <c r="AH207" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="AI207" t="s">
         <v>84</v>
@@ -25199,7 +25193,7 @@
         <v>87</v>
       </c>
       <c r="R219" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="S219" t="s">
         <v>89</v>
@@ -25291,7 +25285,7 @@
         <v>129</v>
       </c>
       <c r="R220" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="S220" t="s">
         <v>89</v>
@@ -25365,7 +25359,7 @@
     </row>
     <row r="221" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B221" t="s">
         <v>106</v>
@@ -25608,7 +25602,7 @@
         <v>87</v>
       </c>
       <c r="V224" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="W224" t="s">
         <v>83</v>
@@ -26087,7 +26081,7 @@
         <v>92</v>
       </c>
       <c r="AR228" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AS228" t="s">
         <v>110</v>
@@ -26161,7 +26155,7 @@
         <v>119</v>
       </c>
       <c r="Z229" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="AA229" t="s">
         <v>116</v>
@@ -26191,7 +26185,7 @@
         <v>97</v>
       </c>
       <c r="AJ229" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="AK229" t="s">
         <v>129</v>
@@ -26464,7 +26458,7 @@
         <v>110</v>
       </c>
       <c r="AL232" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="AM232" t="s">
         <v>87</v>
@@ -26915,7 +26909,7 @@
         <v>87</v>
       </c>
       <c r="P237" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="Q237" t="s">
         <v>87</v>
@@ -26971,7 +26965,7 @@
         <v>87</v>
       </c>
       <c r="P238" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="Q238" t="s">
         <v>87</v>
@@ -27049,7 +27043,7 @@
         <v>116</v>
       </c>
       <c r="AP238" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="AQ238" t="s">
         <v>87</v>
@@ -27165,7 +27159,7 @@
         <v>110</v>
       </c>
       <c r="T239" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="U239" t="s">
         <v>117</v>
@@ -27249,7 +27243,7 @@
         <v>102</v>
       </c>
       <c r="AV239" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="AW239" t="s">
         <v>89</v>
@@ -28145,7 +28139,7 @@
         <v>85</v>
       </c>
       <c r="L249" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="M249" t="s">
         <v>122</v>
@@ -28330,7 +28324,7 @@
         <v>102</v>
       </c>
       <c r="AX250" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="AY250" t="s">
         <v>92</v>
@@ -28544,7 +28538,7 @@
         <v>95</v>
       </c>
       <c r="BD252" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="BE252" t="s">
         <v>87</v>
@@ -28674,7 +28668,7 @@
         <v>95</v>
       </c>
       <c r="V254" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="W254" t="s">
         <v>89</v>
@@ -28727,7 +28721,7 @@
         <v>106</v>
       </c>
       <c r="X255" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="Y255" t="s">
         <v>117</v>
@@ -29167,7 +29161,7 @@
         <v>102</v>
       </c>
       <c r="BF259" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="BG259" t="s">
         <v>89</v>
@@ -29185,13 +29179,13 @@
         <v>95</v>
       </c>
       <c r="BL259" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="BM259" t="s">
         <v>89</v>
       </c>
       <c r="BN259" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="BO259" t="s">
         <v>89</v>
@@ -29265,7 +29259,7 @@
         <v>97</v>
       </c>
       <c r="AD260" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="AE260" t="s">
         <v>129</v>
@@ -29389,7 +29383,7 @@
         <v>122</v>
       </c>
       <c r="N262" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="O262" t="s">
         <v>122</v>
@@ -29974,7 +29968,7 @@
     </row>
     <row r="268" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B268" t="s">
         <v>110</v>
@@ -30634,7 +30628,7 @@
         <v>102</v>
       </c>
       <c r="N274" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="O274" t="s">
         <v>83</v>
@@ -30859,7 +30853,7 @@
         <v>119</v>
       </c>
       <c r="R277" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="S277" t="s">
         <v>117</v>
@@ -30925,7 +30919,7 @@
         <v>117</v>
       </c>
       <c r="AN277" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AO277" t="s">
         <v>110</v>
@@ -31585,7 +31579,7 @@
         <v>102</v>
       </c>
       <c r="BB283" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="BC283" t="s">
         <v>89</v>
@@ -31766,7 +31760,7 @@
         <v>83</v>
       </c>
       <c r="R285" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="S285" t="s">
         <v>97</v>
@@ -31819,7 +31813,7 @@
         <v>92</v>
       </c>
       <c r="N286" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="O286" t="s">
         <v>108</v>
@@ -32822,7 +32816,7 @@
         <v>110</v>
       </c>
       <c r="Z294" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AA294" t="s">
         <v>110</v>
@@ -32926,7 +32920,7 @@
         <v>87</v>
       </c>
       <c r="AJ295" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AK295" t="s">
         <v>110</v>
@@ -33345,7 +33339,7 @@
         <v>127</v>
       </c>
       <c r="N299" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="O299" t="s">
         <v>89</v>
@@ -33440,7 +33434,7 @@
         <v>127</v>
       </c>
       <c r="N300" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="O300" t="s">
         <v>89</v>
@@ -33556,7 +33550,7 @@
         <v>100</v>
       </c>
       <c r="T301" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="U301" t="s">
         <v>89</v>
@@ -34019,7 +34013,7 @@
         <v>85</v>
       </c>
       <c r="L309" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="M309" t="s">
         <v>122</v>
@@ -34129,7 +34123,7 @@
         <v>97</v>
       </c>
       <c r="Z310" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="AA310" t="s">
         <v>129</v>
@@ -34743,7 +34737,7 @@
     </row>
     <row r="317" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B317" t="s">
         <v>129</v>
@@ -34820,7 +34814,7 @@
         <v>85</v>
       </c>
       <c r="L318" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="M318" t="s">
         <v>122</v>
@@ -34963,7 +34957,7 @@
         <v>127</v>
       </c>
       <c r="N319" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="O319" t="s">
         <v>83</v>
@@ -35334,7 +35328,7 @@
         <v>129</v>
       </c>
       <c r="AB323" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="AC323" t="s">
         <v>116</v>
@@ -35569,13 +35563,13 @@
         <v>102</v>
       </c>
       <c r="AL325" t="s">
+        <v>785</v>
+      </c>
+      <c r="AM325" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN325" t="s">
         <v>786</v>
-      </c>
-      <c r="AM325" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN325" t="s">
-        <v>787</v>
       </c>
       <c r="AO325" t="s">
         <v>87</v>
@@ -35869,7 +35863,7 @@
         <v>102</v>
       </c>
       <c r="AL328" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="AM328" t="s">
         <v>89</v>
@@ -36014,7 +36008,7 @@
         <v>97</v>
       </c>
       <c r="X330" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="Y330" t="s">
         <v>110</v>
@@ -36571,7 +36565,7 @@
         <v>127</v>
       </c>
       <c r="P337" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="Q337" t="s">
         <v>97</v>
@@ -36690,7 +36684,7 @@
         <v>129</v>
       </c>
       <c r="AD338" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="AE338" t="s">
         <v>116</v>
@@ -36794,7 +36788,7 @@
         <v>129</v>
       </c>
       <c r="AD339" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="AE339" t="s">
         <v>116</v>
@@ -37145,7 +37139,7 @@
         <v>92</v>
       </c>
       <c r="V342" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="W342" t="s">
         <v>89</v>
@@ -37231,7 +37225,7 @@
         <v>92</v>
       </c>
       <c r="R343" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="S343" t="s">
         <v>89</v>
@@ -38227,7 +38221,7 @@
         <v>87</v>
       </c>
       <c r="V352" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="W352" t="s">
         <v>119</v>
@@ -38325,7 +38319,7 @@
         <v>117</v>
       </c>
       <c r="N353" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="O353" t="s">
         <v>89</v>
@@ -38369,7 +38363,7 @@
         <v>85</v>
       </c>
       <c r="L354" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="M354" t="s">
         <v>122</v>
@@ -38665,7 +38659,7 @@
         <v>110</v>
       </c>
       <c r="T355" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="U355" t="s">
         <v>110</v>
@@ -38791,7 +38785,7 @@
         <v>102</v>
       </c>
       <c r="N358" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="O358" t="s">
         <v>97</v>
@@ -38853,7 +38847,7 @@
         <v>102</v>
       </c>
       <c r="N359" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="O359" t="s">
         <v>97</v>
@@ -38915,7 +38909,7 @@
         <v>102</v>
       </c>
       <c r="N360" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="O360" t="s">
         <v>97</v>
@@ -38977,7 +38971,7 @@
         <v>102</v>
       </c>
       <c r="N361" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="O361" t="s">
         <v>97</v>
@@ -39119,7 +39113,7 @@
         <v>122</v>
       </c>
       <c r="N363" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="O363" t="s">
         <v>122</v>
@@ -39251,7 +39245,7 @@
         <v>87</v>
       </c>
       <c r="BF363" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="BG363" t="s">
         <v>129</v>
@@ -39408,7 +39402,7 @@
         <v>84</v>
       </c>
       <c r="X365" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="Y365" t="s">
         <v>87</v>
@@ -39750,7 +39744,7 @@
         <v>122</v>
       </c>
       <c r="P368" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="Q368" t="s">
         <v>122</v>
@@ -40056,7 +40050,7 @@
         <v>87</v>
       </c>
       <c r="P371" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="Q371" t="s">
         <v>89</v>
@@ -41075,7 +41069,7 @@
     </row>
     <row r="381" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B381" t="s">
         <v>106</v>
@@ -41427,7 +41421,7 @@
         <v>87</v>
       </c>
       <c r="N386" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="O386" t="s">
         <v>100</v>
@@ -41995,13 +41989,13 @@
         <v>116</v>
       </c>
       <c r="R391" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="S391" t="s">
         <v>106</v>
       </c>
       <c r="T391" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="U391" t="s">
         <v>83</v>
@@ -42051,7 +42045,7 @@
     </row>
     <row r="392" spans="1:93" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B392" t="s">
         <v>117</v>
@@ -42132,7 +42126,7 @@
         <v>119</v>
       </c>
       <c r="AJ392" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="AK392" t="s">
         <v>102</v>
@@ -42200,7 +42194,7 @@
         <v>117</v>
       </c>
       <c r="AB393" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="AC393" t="s">
         <v>117</v>
@@ -42483,7 +42477,7 @@
         <v>85</v>
       </c>
       <c r="L395" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="M395" t="s">
         <v>117</v>
@@ -42659,7 +42653,7 @@
         <v>97</v>
       </c>
       <c r="AP396" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="AQ396" t="s">
         <v>129</v>
@@ -42695,7 +42689,7 @@
         <v>84</v>
       </c>
       <c r="BB396" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="BC396" t="s">
         <v>129</v>
@@ -43228,7 +43222,7 @@
         <v>117</v>
       </c>
       <c r="P400" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="Q400" t="s">
         <v>117</v>
@@ -44325,7 +44319,7 @@
         <v>87</v>
       </c>
       <c r="T413" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="U413" t="s">
         <v>83</v>
@@ -45196,7 +45190,7 @@
         <v>95</v>
       </c>
       <c r="X424" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="Y424" t="s">
         <v>89</v>
@@ -46170,7 +46164,7 @@
         <v>102</v>
       </c>
       <c r="N434" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="O434" t="s">
         <v>84</v>
@@ -47080,7 +47074,7 @@
         <v>102</v>
       </c>
       <c r="BB442" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="BC442" t="s">
         <v>92</v>
@@ -47142,7 +47136,7 @@
         <v>117</v>
       </c>
       <c r="V443" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="W443" t="s">
         <v>110</v>
@@ -47164,6 +47158,12 @@
       </c>
       <c r="AC443" t="s">
         <v>110</v>
+      </c>
+      <c r="AD443" t="s">
+        <v>819</v>
+      </c>
+      <c r="AE443" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="444" spans="1:63" x14ac:dyDescent="0.35">
@@ -47240,7 +47240,7 @@
         <v>102</v>
       </c>
       <c r="AF444" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AG444" t="s">
         <v>110</v>
@@ -47308,7 +47308,7 @@
         <v>89</v>
       </c>
       <c r="P445" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="Q445" t="s">
         <v>100</v>
@@ -47370,7 +47370,7 @@
         <v>148</v>
       </c>
       <c r="L446" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="M446" t="s">
         <v>87</v>
@@ -48183,6 +48183,12 @@
       <c r="AQ451" t="s">
         <v>127</v>
       </c>
+      <c r="AR451" t="s">
+        <v>808</v>
+      </c>
+      <c r="AS451" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="452" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A452" t="s">
@@ -48414,7 +48420,7 @@
         <v>222</v>
       </c>
       <c r="M455" t="s">
-        <v>119</v>
+        <v>222</v>
       </c>
       <c r="N455" t="s">
         <v>204</v>
@@ -48435,7 +48441,7 @@
         <v>106</v>
       </c>
       <c r="T455" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="U455" t="s">
         <v>92</v>
@@ -48618,7 +48624,7 @@
         <v>83</v>
       </c>
       <c r="X458" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="Y458" t="s">
         <v>110</v>
@@ -48712,7 +48718,7 @@
         <v>95</v>
       </c>
       <c r="R460" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="S460" t="s">
         <v>110</v>
@@ -48818,7 +48824,7 @@
         <v>83</v>
       </c>
       <c r="P462" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="Q462" t="s">
         <v>116</v>
@@ -49745,7 +49751,7 @@
         <v>95</v>
       </c>
       <c r="X474" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="Y474" t="s">
         <v>119</v>
@@ -49861,7 +49867,7 @@
         <v>102</v>
       </c>
       <c r="AP475" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="AQ475" t="s">
         <v>110</v>
@@ -49915,7 +49921,7 @@
         <v>117</v>
       </c>
       <c r="BH475" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="BI475" t="s">
         <v>110</v>
@@ -50161,7 +50167,7 @@
         <v>85</v>
       </c>
       <c r="L481" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="M481" t="s">
         <v>122</v>
@@ -50309,7 +50315,7 @@
         <v>87</v>
       </c>
       <c r="V483" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="W483" t="s">
         <v>89</v>
@@ -50517,7 +50523,7 @@
         <v>83</v>
       </c>
       <c r="X485" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="Y485" t="s">
         <v>110</v>
@@ -50762,7 +50768,7 @@
         <v>102</v>
       </c>
       <c r="CF486" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="CG486" t="s">
         <v>102</v>
@@ -50877,7 +50883,7 @@
         <v>87</v>
       </c>
       <c r="P488" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="Q488" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Move details till fire fang
</commit_message>
<xml_diff>
--- a/Pokemon.xlsx
+++ b/Pokemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijan Badhya\Documents\Pokemon_elite_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65D62C7-D4F3-426B-836F-B586B7D7843A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4D4C44-A631-4234-B2B5-9AC724BABC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2870,8 +2870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CS489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="99" workbookViewId="0">
-      <selection activeCell="M130" sqref="M130"/>
+    <sheetView tabSelected="1" topLeftCell="A375" zoomScale="99" workbookViewId="0">
+      <selection activeCell="N386" sqref="N386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Move details Jaw Lock
</commit_message>
<xml_diff>
--- a/Pokemon.xlsx
+++ b/Pokemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijan Badhya\Documents\Pokemon_elite_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4D4C44-A631-4234-B2B5-9AC724BABC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1E1B0C-9A81-4155-9735-284F83823376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15380" uniqueCount="820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30771" uniqueCount="821">
   <si>
     <t>Name</t>
   </si>
@@ -2483,6 +2483,9 @@
   </si>
   <si>
     <t>Snarl</t>
+  </si>
+  <si>
+    <t>Air Cutter</t>
   </si>
 </sst>
 </file>
@@ -2870,8 +2873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CS489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A375" zoomScale="99" workbookViewId="0">
-      <selection activeCell="N386" sqref="N386"/>
+    <sheetView tabSelected="1" topLeftCell="AA210" zoomScale="99" workbookViewId="0">
+      <selection activeCell="AR222" sqref="AR222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25469,6 +25472,12 @@
       <c r="AQ221" t="s">
         <v>116</v>
       </c>
+      <c r="AR221" t="s">
+        <v>820</v>
+      </c>
+      <c r="AS221" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="222" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A222" t="s">

</xml_diff>

<commit_message>
Move details till Surf
</commit_message>
<xml_diff>
--- a/Pokemon.xlsx
+++ b/Pokemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijan Badhya\Documents\Pokemon_elite_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1E1B0C-9A81-4155-9735-284F83823376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05781DE1-8970-4049-AAC4-936DB40CE78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30771" uniqueCount="821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15382" uniqueCount="821">
   <si>
     <t>Name</t>
   </si>
@@ -2873,8 +2873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CS489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA210" zoomScale="99" workbookViewId="0">
-      <selection activeCell="AR222" sqref="AR222"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="99" workbookViewId="0">
+      <selection activeCell="G111" sqref="G111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13290,7 +13290,7 @@
         <v>89</v>
       </c>
       <c r="E110">
-        <v>56</v>
+        <v>161</v>
       </c>
       <c r="F110">
         <v>50</v>

</xml_diff>

<commit_message>
successfully implemented atk spa formula
</commit_message>
<xml_diff>
--- a/Pokemon.xlsx
+++ b/Pokemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijan Badhya\Documents\Pokemon_elite_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05781DE1-8970-4049-AAC4-936DB40CE78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDD6E9E-41D6-4C65-A377-58004906560A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2873,8 +2873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CS489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="99" workbookViewId="0">
-      <selection activeCell="G111" sqref="G111"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="99" workbookViewId="0">
+      <selection activeCell="E176" sqref="E176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
merged filtering with formula
</commit_message>
<xml_diff>
--- a/Pokemon.xlsx
+++ b/Pokemon.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijan Badhya\Documents\Pokemon_elite_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7456495-378D-4FCF-99A2-E0FAFD638DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78962FCF-2A1A-4010-AC13-E3C64863E135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2873,8 +2873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CS489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A391" zoomScale="99" workbookViewId="0">
-      <selection activeCell="I410" sqref="I410"/>
+    <sheetView tabSelected="1" topLeftCell="A486" zoomScale="99" workbookViewId="0">
+      <selection activeCell="H489" sqref="H489"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
made movesdf and typedf obsolete
</commit_message>
<xml_diff>
--- a/Pokemon.xlsx
+++ b/Pokemon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijan Badhya\Documents\Pokemon_elite_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78962FCF-2A1A-4010-AC13-E3C64863E135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FAFBD4-C09B-4906-A8C1-75C513E15FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15384" uniqueCount="821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15387" uniqueCount="821">
   <si>
     <t>Name</t>
   </si>
@@ -2873,8 +2873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CS489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A486" zoomScale="99" workbookViewId="0">
-      <selection activeCell="H489" sqref="H489"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="99" workbookViewId="0">
+      <selection activeCell="M119" sqref="M119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -31310,6 +31310,9 @@
       <c r="H275" t="s">
         <v>85</v>
       </c>
+      <c r="J275" t="s">
+        <v>148</v>
+      </c>
       <c r="L275" t="s">
         <v>199</v>
       </c>
@@ -38223,6 +38226,9 @@
       <c r="H343" t="s">
         <v>85</v>
       </c>
+      <c r="J343" t="s">
+        <v>148</v>
+      </c>
       <c r="L343" t="s">
         <v>93</v>
       </c>
@@ -40242,6 +40248,9 @@
       </c>
       <c r="H363" t="s">
         <v>85</v>
+      </c>
+      <c r="J363" t="s">
+        <v>148</v>
       </c>
       <c r="L363" t="s">
         <v>121</v>

</xml_diff>